<commit_message>
finalizing MachineIBR examples and slides
</commit_message>
<xml_diff>
--- a/emt-bootcamp/Support/EMTBootCamp.xlsx
+++ b/emt-bootcamp/Support/EMTBootCamp.xlsx
@@ -8,26 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\i2x\emt-bootcamp\Support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D2AF2A-0D52-4A82-AFED-5BF4301E261E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6268B7-53E3-4D93-9CF8-E07BC7499398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="2220" windowWidth="28800" windowHeight="15450" xr2:uid="{A8C2E3F1-142E-440E-A762-DE7B4CF8E5D3}"/>
+    <workbookView xWindow="7200" yWindow="4230" windowWidth="28800" windowHeight="15450" activeTab="1" xr2:uid="{A8C2E3F1-142E-440E-A762-DE7B4CF8E5D3}"/>
   </bookViews>
   <sheets>
     <sheet name="COMTRADE" sheetId="1" r:id="rId1"/>
     <sheet name="Source" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Dmax">COMTRADE!$M$2</definedName>
-    <definedName name="Dmin">COMTRADE!$M$1</definedName>
-    <definedName name="Ibase">COMTRADE!$M$5</definedName>
-    <definedName name="IpuMax">COMTRADE!$M$10</definedName>
-    <definedName name="Iscale">COMTRADE!$M$7</definedName>
-    <definedName name="Splant">COMTRADE!$M$3</definedName>
-    <definedName name="SpuMax">COMTRADE!$M$11</definedName>
-    <definedName name="Sscale">COMTRADE!$M$8</definedName>
-    <definedName name="Vpoc">COMTRADE!$M$4</definedName>
-    <definedName name="VpuMax">COMTRADE!$M$9</definedName>
-    <definedName name="Vscale">COMTRADE!$M$6</definedName>
+    <definedName name="Dmax">COMTRADE!$N$2</definedName>
+    <definedName name="Dmin">COMTRADE!$N$1</definedName>
+    <definedName name="Ibase">COMTRADE!$N$5</definedName>
+    <definedName name="IpuMax">COMTRADE!$N$10</definedName>
+    <definedName name="Iscale">COMTRADE!$N$7</definedName>
+    <definedName name="Splant">COMTRADE!$N$3</definedName>
+    <definedName name="SpuMax">COMTRADE!$N$11</definedName>
+    <definedName name="Sscale">COMTRADE!$N$8</definedName>
+    <definedName name="Vpoc">COMTRADE!$N$4</definedName>
+    <definedName name="VpuMax">COMTRADE!$N$9</definedName>
+    <definedName name="Vscale">COMTRADE!$N$6</definedName>
     <definedName name="XS">Source!$F$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -51,10 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
-  <si>
-    <t>Index</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -89,15 +86,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>Units</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
     <t>kV</t>
   </si>
   <si>
@@ -116,27 +104,12 @@
     <t>MW</t>
   </si>
   <si>
-    <t>MVAR</t>
-  </si>
-  <si>
     <t>Hz</t>
   </si>
   <si>
     <t>A</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>Vpu</t>
-  </si>
-  <si>
-    <t>Xf</t>
-  </si>
-  <si>
-    <t>Lf</t>
-  </si>
-  <si>
     <t>Zs</t>
   </si>
   <si>
@@ -185,21 +158,97 @@
     <t>SpuMax</t>
   </si>
   <si>
-    <t>Primary</t>
-  </si>
-  <si>
-    <t>Secondary</t>
+    <r>
+      <t>Xf [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>Lf [H]</t>
+  </si>
+  <si>
+    <t>Vf [pu]</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>var</t>
+  </si>
+  <si>
+    <t>PSCAD
+Units</t>
+  </si>
+  <si>
+    <t>EMTP
+Units</t>
+  </si>
+  <si>
+    <t>PSCAD
+Index</t>
+  </si>
+  <si>
+    <t>EMTP
+Min</t>
+  </si>
+  <si>
+    <t>EMTP
+Max</t>
+  </si>
+  <si>
+    <t>EMTP
+A</t>
+  </si>
+  <si>
+    <t>EMTP
+B</t>
+  </si>
+  <si>
+    <t>EMTP
+Primary</t>
+  </si>
+  <si>
+    <t>EMTP
+Secondary</t>
+  </si>
+  <si>
+    <t>Mvar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0E+00"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +263,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -242,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -268,17 +325,29 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,472 +662,510 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2EFB84-5509-400E-9C84-8F084E94ECFC}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="11.6328125" customWidth="1"/>
-    <col min="7" max="7" width="13.81640625" customWidth="1"/>
-    <col min="10" max="10" width="10.453125" customWidth="1"/>
+    <col min="4" max="4" width="8.7265625" customWidth="1"/>
+    <col min="5" max="5" width="7.6328125" customWidth="1"/>
+    <col min="6" max="6" width="8.54296875" customWidth="1"/>
+    <col min="7" max="7" width="8.6328125" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="11" max="11" width="10.453125" customWidth="1"/>
+    <col min="12" max="12" width="5.81640625" customWidth="1"/>
+    <col min="13" max="13" width="9.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="D1" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="9">
+        <v>-32767</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="L1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M1" s="9">
-        <v>-32767</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="5">
-        <f>-F2</f>
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="16">
+        <f>-G2</f>
         <v>-375588.42722675402</v>
       </c>
-      <c r="F2" s="4">
+      <c r="G2" s="17">
         <f>SQRT(2)*Vpoc*Vscale*VpuMax/SQRT(3)</f>
         <v>375588.42722675402</v>
       </c>
-      <c r="G2" s="5">
-        <f t="shared" ref="G2:G11" si="0">(F2-E2)/(Dmax-Dmin)</f>
+      <c r="H2" s="5">
+        <f t="shared" ref="H2:H11" si="0">(G2-F2)/(Dmax-Dmin)</f>
         <v>11.462398975394574</v>
       </c>
-      <c r="H2" s="5">
-        <f t="shared" ref="H2:H11" si="1">F2-G2*Dmax</f>
+      <c r="I2" s="5">
+        <f t="shared" ref="I2:I11" si="1">G2-H2*Dmax</f>
         <v>0</v>
       </c>
-      <c r="I2" s="14">
+      <c r="J2" s="12">
         <v>1000</v>
       </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="L2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" s="9">
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="9">
         <v>32767</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="5">
-        <f t="shared" ref="E3:E7" si="2">-F3</f>
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="16">
+        <f t="shared" ref="F3:F7" si="2">-G3</f>
         <v>-375588.42722675402</v>
       </c>
-      <c r="F3" s="5">
-        <f>F$2</f>
+      <c r="G3" s="16">
+        <f>G$2</f>
         <v>375588.42722675402</v>
       </c>
-      <c r="G3" s="5">
+      <c r="H3" s="5">
         <f t="shared" si="0"/>
         <v>11.462398975394574</v>
       </c>
-      <c r="H3" s="5">
+      <c r="I3" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I3" s="14">
+      <c r="J3" s="12">
         <v>1000</v>
       </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="10">
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="10">
         <v>100000000</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="5">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="16">
         <f t="shared" si="2"/>
         <v>-375588.42722675402</v>
       </c>
-      <c r="F4" s="5">
-        <f>F$2</f>
+      <c r="G4" s="16">
+        <f>G$2</f>
         <v>375588.42722675402</v>
       </c>
-      <c r="G4" s="5">
+      <c r="H4" s="5">
         <f t="shared" si="0"/>
         <v>11.462398975394574</v>
       </c>
-      <c r="H4" s="5">
+      <c r="I4" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I4" s="14">
+      <c r="J4" s="12">
         <v>1000</v>
       </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" s="10">
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="M4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="10">
         <v>230000</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="5">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="16">
         <f t="shared" si="2"/>
         <v>-2129.9910806810249</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="17">
         <f>SQRT(2)*Ibase*Iscale*IpuMax</f>
         <v>2129.9910806810249</v>
       </c>
-      <c r="G5" s="5">
+      <c r="H5" s="5">
         <f t="shared" si="0"/>
         <v>6.5004152979553351E-2</v>
       </c>
-      <c r="H5" s="5">
+      <c r="I5" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I5" s="14">
+      <c r="J5" s="12">
         <v>1000</v>
       </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="L5" t="s">
-        <v>37</v>
-      </c>
-      <c r="M5">
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="M5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5">
         <f>Splant/SQRT(3)/Vpoc</f>
         <v>251.02185616940253</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="5">
+        <v>12</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="16">
         <f t="shared" si="2"/>
         <v>-2129.9910806810249</v>
       </c>
-      <c r="F6" s="5">
-        <f>F$5</f>
+      <c r="G6" s="16">
+        <f>G$5</f>
         <v>2129.9910806810249</v>
       </c>
-      <c r="G6" s="5">
+      <c r="H6" s="5">
         <f t="shared" si="0"/>
         <v>6.5004152979553351E-2</v>
       </c>
-      <c r="H6" s="5">
+      <c r="I6" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I6" s="14">
+      <c r="J6" s="12">
         <v>1000</v>
       </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="L6" t="s">
-        <v>38</v>
-      </c>
-      <c r="M6" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="M6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="5">
+        <v>12</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="16">
         <f t="shared" si="2"/>
         <v>-2129.9910806810249</v>
       </c>
-      <c r="F7" s="5">
-        <f>F$5</f>
+      <c r="G7" s="16">
+        <f>G$5</f>
         <v>2129.9910806810249</v>
       </c>
-      <c r="G7" s="5">
+      <c r="H7" s="5">
         <f t="shared" si="0"/>
         <v>6.5004152979553351E-2</v>
       </c>
-      <c r="H7" s="5">
+      <c r="I7" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I7" s="14">
+      <c r="J7" s="12">
         <v>1000</v>
       </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="L7" t="s">
-        <v>39</v>
-      </c>
-      <c r="M7" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="M7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="5">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="16">
         <v>0</v>
       </c>
-      <c r="F8" s="4">
+      <c r="G8" s="17">
         <f>Vpoc*Vscale*VpuMax/SQRT(3)</f>
         <v>265581.12382722786</v>
       </c>
-      <c r="G8" s="5">
+      <c r="H8" s="5">
         <f t="shared" si="0"/>
         <v>4.0525700220836187</v>
       </c>
-      <c r="H8" s="5">
+      <c r="I8" s="5">
         <f t="shared" si="1"/>
         <v>132790.56191361393</v>
       </c>
-      <c r="I8" s="14">
+      <c r="J8" s="12">
         <v>1000</v>
       </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-      <c r="L8" t="s">
-        <v>40</v>
-      </c>
-      <c r="M8" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="M8" t="s">
+        <v>31</v>
+      </c>
+      <c r="N8" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="5">
-        <f>-F9</f>
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="19">
+        <f>-G9</f>
         <v>-300000000</v>
       </c>
-      <c r="F9" s="12">
+      <c r="G9" s="18">
         <f>Splant*Sscale*SpuMax</f>
         <v>300000000</v>
       </c>
-      <c r="G9" s="5">
+      <c r="H9" s="5">
         <f t="shared" si="0"/>
         <v>9155.5528427991576</v>
       </c>
-      <c r="H9" s="5">
+      <c r="I9" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I9" s="14">
+      <c r="J9" s="12">
         <v>1000000</v>
       </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="L9" t="s">
-        <v>41</v>
-      </c>
-      <c r="M9" s="9">
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="M9" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9" s="9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="5">
-        <f>-F10</f>
+        <v>50</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="19">
+        <f>-G10</f>
         <v>-300000000</v>
       </c>
-      <c r="F10" s="13">
-        <f>F$9</f>
+      <c r="G10" s="19">
+        <f>G$9</f>
         <v>300000000</v>
       </c>
-      <c r="G10" s="5">
+      <c r="H10" s="5">
         <f t="shared" si="0"/>
         <v>9155.5528427991576</v>
       </c>
-      <c r="H10" s="5">
+      <c r="I10" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I10" s="14">
+      <c r="J10" s="12">
         <v>1000000</v>
       </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="L10" t="s">
-        <v>42</v>
-      </c>
-      <c r="M10" s="9">
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="M10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N10" s="9">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="11">
+        <v>17</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="13">
         <v>55</v>
       </c>
-      <c r="F11" s="11">
+      <c r="G11" s="13">
         <v>65</v>
       </c>
-      <c r="G11" s="5">
+      <c r="H11" s="5">
         <f t="shared" si="0"/>
         <v>1.5259254737998596E-4</v>
       </c>
-      <c r="H11" s="5">
+      <c r="I11" s="5">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="I11" s="14">
-        <v>1</v>
-      </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="L11" t="s">
-        <v>43</v>
-      </c>
-      <c r="M11" s="9">
+      <c r="J11" s="12">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="M11" t="s">
+        <v>34</v>
+      </c>
+      <c r="N11" s="9">
         <v>3</v>
       </c>
     </row>
@@ -1072,27 +1179,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7143908-12DE-459A-B5BB-96ECEF0A7C1B}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F1">
         <v>10</v>
@@ -1111,7 +1219,7 @@
         <v>2.6691803111656499E-4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="F2">
         <v>85</v>
@@ -1130,7 +1238,7 @@
         <v>8.8082950268466454E-3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F3">
         <f>$F$2*PI()/180</f>
@@ -1150,7 +1258,7 @@
         <v>2.6424885080539934E-2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F4">
         <f>$F$1*COS($F$3)</f>
@@ -1170,7 +1278,7 @@
         <v>0.10569954032215975</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F5">
         <f>$F$1*SIN($F$3)</f>
@@ -1179,5 +1287,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
automating model initialization tests in PSCAD
</commit_message>
<xml_diff>
--- a/emt-bootcamp/Support/EMTBootCamp.xlsx
+++ b/emt-bootcamp/Support/EMTBootCamp.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\i2x\emt-bootcamp\Support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6268B7-53E3-4D93-9CF8-E07BC7499398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD34864B-4B2E-4B95-BB91-2CD1CDAF1002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="4230" windowWidth="28800" windowHeight="15450" activeTab="1" xr2:uid="{A8C2E3F1-142E-440E-A762-DE7B4CF8E5D3}"/>
+    <workbookView xWindow="5000" yWindow="3220" windowWidth="22660" windowHeight="12780" activeTab="2" xr2:uid="{A8C2E3F1-142E-440E-A762-DE7B4CF8E5D3}"/>
   </bookViews>
   <sheets>
     <sheet name="COMTRADE" sheetId="1" r:id="rId1"/>
     <sheet name="Source" sheetId="2" r:id="rId2"/>
+    <sheet name="Weak" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Dmax">COMTRADE!$N$2</definedName>
@@ -28,6 +29,7 @@
     <definedName name="Vpoc">COMTRADE!$N$4</definedName>
     <definedName name="VpuMax">COMTRADE!$N$9</definedName>
     <definedName name="Vscale">COMTRADE!$N$6</definedName>
+    <definedName name="XS" localSheetId="2">Weak!$F$5</definedName>
     <definedName name="XS">Source!$F$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -51,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -238,6 +240,18 @@
   <si>
     <t>Mvar</t>
   </si>
+  <si>
+    <t>SC MVA</t>
+  </si>
+  <si>
+    <t>IBR MVA</t>
+  </si>
+  <si>
+    <t>SCR</t>
+  </si>
+  <si>
+    <t>kVs</t>
+  </si>
 </sst>
 </file>
 
@@ -246,7 +260,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0E+00"/>
+    <numFmt numFmtId="166" formatCode="0E+00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -326,7 +340,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -342,10 +356,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1177,10 +1191,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7143908-12DE-459A-B5BB-96ECEF0A7C1B}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1285,6 +1299,190 @@
         <v>9.961946980917455</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7">
+        <f>F6*F6/F1</f>
+        <v>5290</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9">
+        <f>F7/F8</f>
+        <v>52.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE8CDAB3-5235-4A87-8D47-F5FCC0EB49C6}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1">
+        <v>211.6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="B2" s="7">
+        <f>XS*A2/(1-A2)</f>
+        <v>2.1292403850122561</v>
+      </c>
+      <c r="C2" s="8">
+        <f>B2/120/PI()</f>
+        <v>5.6479855384265155E-3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="B3" s="7">
+        <f>XS*A3/(1-A3)</f>
+        <v>70.264932705404448</v>
+      </c>
+      <c r="C3" s="8">
+        <f t="shared" ref="C3:C5" si="0">B3/120/PI()</f>
+        <v>0.18638352276807502</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3">
+        <f>$F$2*PI()/180</f>
+        <v>1.4835298641951802</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="B4" s="7">
+        <f>XS*A4/(1-A4)</f>
+        <v>210.79479811621334</v>
+      </c>
+      <c r="C4" s="8">
+        <f t="shared" si="0"/>
+        <v>0.55915056830422505</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <f>$F$1*COS($F$3)</f>
+        <v>18.442155165404461</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="B5" s="7">
+        <f>XS*A5/(1-A5)</f>
+        <v>843.1791924648536</v>
+      </c>
+      <c r="C5" s="8">
+        <f t="shared" si="0"/>
+        <v>2.2366022732169006</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5">
+        <f>$F$1*SIN($F$3)</f>
+        <v>210.79479811621334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7">
+        <f>F6*F6/F1</f>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9">
+        <f>F7/F8</f>
+        <v>2.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
finished the PSCAD plant model tests, except for the SCR ramp
</commit_message>
<xml_diff>
--- a/emt-bootcamp/Support/EMTBootCamp.xlsx
+++ b/emt-bootcamp/Support/EMTBootCamp.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\i2x\emt-bootcamp\Support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD34864B-4B2E-4B95-BB91-2CD1CDAF1002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F0DED8-509C-4DC8-8BE5-148448A10062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5000" yWindow="3220" windowWidth="22660" windowHeight="12780" activeTab="2" xr2:uid="{A8C2E3F1-142E-440E-A762-DE7B4CF8E5D3}"/>
+    <workbookView xWindow="11960" yWindow="2290" windowWidth="22660" windowHeight="12780" activeTab="3" xr2:uid="{A8C2E3F1-142E-440E-A762-DE7B4CF8E5D3}"/>
   </bookViews>
   <sheets>
     <sheet name="COMTRADE" sheetId="1" r:id="rId1"/>
     <sheet name="Source" sheetId="2" r:id="rId2"/>
     <sheet name="Weak" sheetId="3" r:id="rId3"/>
+    <sheet name="StepSCR" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Dmax">COMTRADE!$N$2</definedName>
@@ -29,6 +30,7 @@
     <definedName name="Vpoc">COMTRADE!$N$4</definedName>
     <definedName name="VpuMax">COMTRADE!$N$9</definedName>
     <definedName name="Vscale">COMTRADE!$N$6</definedName>
+    <definedName name="XS" localSheetId="3">StepSCR!$F$5</definedName>
     <definedName name="XS" localSheetId="2">Weak!$F$5</definedName>
     <definedName name="XS">Source!$F$5</definedName>
   </definedNames>
@@ -53,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -252,15 +254,107 @@
   <si>
     <t>kVs</t>
   </si>
+  <si>
+    <r>
+      <t>X1 [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>SCMVA</t>
+  </si>
+  <si>
+    <r>
+      <t>Xs [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Xt [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <t>Xt [pu]</t>
+  </si>
+  <si>
+    <t>SCR Xt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0E+00"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -313,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -362,6 +456,14 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1343,7 +1445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE8CDAB3-5235-4A87-8D47-F5FCC0EB49C6}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -1487,4 +1589,210 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70A51ED4-A577-4B06-8042-A04C86E2D43B}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="6">
+        <v>20</v>
+      </c>
+      <c r="B2" s="21">
+        <f>A2*F$2</f>
+        <v>2000</v>
+      </c>
+      <c r="C2" s="20">
+        <f>F$1*F$1/B2</f>
+        <v>26.45</v>
+      </c>
+      <c r="D2" s="22">
+        <f>C2-F$4</f>
+        <v>-37.03</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
+        <v>10</v>
+      </c>
+      <c r="B3" s="21">
+        <f t="shared" ref="B3:B9" si="0">A3*F$2</f>
+        <v>1000</v>
+      </c>
+      <c r="C3" s="20">
+        <f t="shared" ref="C3:C9" si="1">F$1*F$1/B3</f>
+        <v>52.9</v>
+      </c>
+      <c r="D3" s="22">
+        <f>C3-F$4</f>
+        <v>-10.579999999999998</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <v>5</v>
+      </c>
+      <c r="B4" s="21">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="C4" s="20">
+        <f t="shared" si="1"/>
+        <v>105.8</v>
+      </c>
+      <c r="D4" s="22">
+        <f t="shared" ref="D3:D9" si="2">C4-F$4</f>
+        <v>42.32</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4">
+        <f>F1*F1*F3/F2</f>
+        <v>63.48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="21">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="C5" s="20">
+        <f t="shared" si="1"/>
+        <v>132.25</v>
+      </c>
+      <c r="D5" s="22">
+        <f t="shared" si="2"/>
+        <v>68.77000000000001</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="23">
+        <f>1/F3</f>
+        <v>8.3333333333333339</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="21">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="C6" s="20">
+        <f t="shared" si="1"/>
+        <v>176.33333333333334</v>
+      </c>
+      <c r="D6" s="22">
+        <f t="shared" si="2"/>
+        <v>112.85333333333335</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="B7" s="21">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="C7" s="20">
+        <f t="shared" si="1"/>
+        <v>211.6</v>
+      </c>
+      <c r="D7" s="22">
+        <f t="shared" si="2"/>
+        <v>148.12</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="6">
+        <v>2</v>
+      </c>
+      <c r="B8" s="21">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="C8" s="20">
+        <f t="shared" si="1"/>
+        <v>264.5</v>
+      </c>
+      <c r="D8" s="22">
+        <f t="shared" si="2"/>
+        <v>201.02</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="6">
+        <v>1</v>
+      </c>
+      <c r="B9" s="21">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="C9" s="20">
+        <f t="shared" si="1"/>
+        <v>529</v>
+      </c>
+      <c r="D9" s="22">
+        <f t="shared" si="2"/>
+        <v>465.52</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
working on EMTP ov, ofuf, angle, and rampscr tests
</commit_message>
<xml_diff>
--- a/emt-bootcamp/Support/EMTBootCamp.xlsx
+++ b/emt-bootcamp/Support/EMTBootCamp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\i2x\emt-bootcamp\Support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00F0DED8-509C-4DC8-8BE5-148448A10062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB5BBD1-59E4-479D-8D60-D921682306E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11960" yWindow="2290" windowWidth="22660" windowHeight="12780" activeTab="3" xr2:uid="{A8C2E3F1-142E-440E-A762-DE7B4CF8E5D3}"/>
+    <workbookView xWindow="850" yWindow="3100" windowWidth="9050" windowHeight="12780" activeTab="3" xr2:uid="{A8C2E3F1-142E-440E-A762-DE7B4CF8E5D3}"/>
   </bookViews>
   <sheets>
     <sheet name="COMTRADE" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="Vpoc">COMTRADE!$N$4</definedName>
     <definedName name="VpuMax">COMTRADE!$N$9</definedName>
     <definedName name="Vscale">COMTRADE!$N$6</definedName>
-    <definedName name="XS" localSheetId="3">StepSCR!$F$5</definedName>
+    <definedName name="XS" localSheetId="3">StepSCR!$H$5</definedName>
     <definedName name="XS" localSheetId="2">Weak!$F$5</definedName>
     <definedName name="XS">Source!$F$5</definedName>
   </definedNames>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -343,6 +343,60 @@
   </si>
   <si>
     <t>SCR Xt</t>
+  </si>
+  <si>
+    <r>
+      <t>Zs [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Rs [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1593,19 +1647,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70A51ED4-A577-4B06-8042-A04C86E2D43B}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.54296875" customWidth="1"/>
+    <col min="4" max="6" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>53</v>
       </c>
@@ -1616,62 +1670,72 @@
         <v>55</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F1">
+      <c r="H1">
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>20</v>
       </c>
       <c r="B2" s="21">
-        <f>A2*F$2</f>
+        <f>A2*H$2</f>
         <v>2000</v>
       </c>
       <c r="C2" s="20">
-        <f>F$1*F$1/B2</f>
+        <f>H$1*H$1/B2</f>
         <v>26.45</v>
       </c>
       <c r="D2" s="22">
-        <f>C2-F$4</f>
+        <f>C2-H$4</f>
         <v>-37.03</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>10</v>
       </c>
       <c r="B3" s="21">
-        <f t="shared" ref="B3:B9" si="0">A3*F$2</f>
+        <f t="shared" ref="B3:B9" si="0">A3*H$2</f>
         <v>1000</v>
       </c>
       <c r="C3" s="20">
-        <f t="shared" ref="C3:C9" si="1">F$1*F$1/B3</f>
+        <f t="shared" ref="C3:C9" si="1">H$1*H$1/B3</f>
         <v>52.9</v>
       </c>
       <c r="D3" s="22">
-        <f>C3-F$4</f>
+        <f>C3-H$4</f>
         <v>-10.579999999999998</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>0.12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>5</v>
       </c>
@@ -1684,18 +1748,26 @@
         <v>105.8</v>
       </c>
       <c r="D4" s="22">
-        <f t="shared" ref="D3:D9" si="2">C4-F$4</f>
+        <f t="shared" ref="D4:D9" si="2">C4-H$4</f>
         <v>42.32</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="22">
+        <f>D4*COS(85/57.2957)</f>
+        <v>3.6883442364681684</v>
+      </c>
+      <c r="F4" s="22">
+        <f>D4*SIN(85/57.2957)</f>
+        <v>42.158967216872284</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F4">
-        <f>F1*F1*F3/F2</f>
+      <c r="H4">
+        <f>H1*H1*H3/H2</f>
         <v>63.48</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1711,15 +1783,23 @@
         <f t="shared" si="2"/>
         <v>68.77000000000001</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="22">
+        <f t="shared" ref="E5:E9" si="3">D5*COS(85/57.2957)</f>
+        <v>5.9935593842607746</v>
+      </c>
+      <c r="F5" s="22">
+        <f t="shared" ref="F5:F9" si="4">D5*SIN(85/57.2957)</f>
+        <v>68.508321727417467</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="23">
-        <f>1/F3</f>
+      <c r="H5" s="23">
+        <f>1/H3</f>
         <v>8.3333333333333339</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>3</v>
       </c>
@@ -1735,9 +1815,17 @@
         <f t="shared" si="2"/>
         <v>112.85333333333335</v>
       </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E6" s="22">
+        <f t="shared" si="3"/>
+        <v>9.8355846305817849</v>
+      </c>
+      <c r="F6" s="22">
+        <f t="shared" si="4"/>
+        <v>112.42391257832611</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>2.5</v>
       </c>
@@ -1753,9 +1841,17 @@
         <f t="shared" si="2"/>
         <v>148.12</v>
       </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E7" s="22">
+        <f t="shared" si="3"/>
+        <v>12.90920482763859</v>
+      </c>
+      <c r="F7" s="22">
+        <f t="shared" si="4"/>
+        <v>147.556385259053</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>2</v>
       </c>
@@ -1771,9 +1867,17 @@
         <f t="shared" si="2"/>
         <v>201.02</v>
       </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="E8" s="22">
+        <f t="shared" si="3"/>
+        <v>17.5196351232238</v>
+      </c>
+      <c r="F8" s="22">
+        <f t="shared" si="4"/>
+        <v>200.25509428014337</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>1</v>
       </c>
@@ -1789,7 +1893,15 @@
         <f t="shared" si="2"/>
         <v>465.52</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="22">
+        <f t="shared" si="3"/>
+        <v>40.571786601149853</v>
+      </c>
+      <c r="F9" s="22">
+        <f t="shared" si="4"/>
+        <v>463.74863938559508</v>
+      </c>
+      <c r="G9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated the SCR ramping impedances
</commit_message>
<xml_diff>
--- a/emt-bootcamp/Support/EMTBootCamp.xlsx
+++ b/emt-bootcamp/Support/EMTBootCamp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\i2x\emt-bootcamp\Support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB5BBD1-59E4-479D-8D60-D921682306E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25267ACC-00E8-4742-ADC0-E9C373FC30C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="850" yWindow="3100" windowWidth="9050" windowHeight="12780" activeTab="3" xr2:uid="{A8C2E3F1-142E-440E-A762-DE7B4CF8E5D3}"/>
+    <workbookView xWindow="440" yWindow="3740" windowWidth="20210" windowHeight="10660" activeTab="3" xr2:uid="{A8C2E3F1-142E-440E-A762-DE7B4CF8E5D3}"/>
   </bookViews>
   <sheets>
     <sheet name="COMTRADE" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="Vpoc">COMTRADE!$N$4</definedName>
     <definedName name="VpuMax">COMTRADE!$N$9</definedName>
     <definedName name="Vscale">COMTRADE!$N$6</definedName>
-    <definedName name="XS" localSheetId="3">StepSCR!$H$5</definedName>
+    <definedName name="XS" localSheetId="3">StepSCR!$J$6</definedName>
     <definedName name="XS" localSheetId="2">Weak!$F$5</definedName>
     <definedName name="XS">Source!$F$5</definedName>
   </definedNames>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -312,91 +312,16 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Xt [</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>W</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>]</t>
-    </r>
-  </si>
-  <si>
-    <t>Xt [pu]</t>
-  </si>
-  <si>
-    <t>SCR Xt</t>
-  </si>
-  <si>
-    <r>
-      <t>Zs [</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>W</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Rs [</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Symbol"/>
-        <family val="1"/>
-        <charset val="2"/>
-      </rPr>
-      <t>W</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>]</t>
-    </r>
+    <t>Xplant</t>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t>SCR Xplant</t>
   </si>
 </sst>
 </file>
@@ -461,7 +386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -518,6 +443,9 @@
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1500,7 +1428,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1647,261 +1575,356 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70A51ED4-A577-4B06-8042-A04C86E2D43B}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="9.54296875" customWidth="1"/>
+    <col min="4" max="4" width="9.36328125" customWidth="1"/>
+    <col min="5" max="8" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="6">
+        <v>20</v>
+      </c>
+      <c r="B3" s="21">
+        <f>A3*J$3</f>
+        <v>2000</v>
+      </c>
+      <c r="C3" s="20">
+        <f>J$2*J$2/B3</f>
+        <v>26.45</v>
+      </c>
+      <c r="D3" s="24">
+        <v>74.06</v>
+      </c>
+      <c r="E3" s="22">
+        <f>C3-D3</f>
+        <v>-47.61</v>
+      </c>
+      <c r="F3" s="24">
+        <v>100.13</v>
+      </c>
+      <c r="G3" s="22">
+        <f>C3-F3</f>
+        <v>-73.679999999999993</v>
+      </c>
+      <c r="H3" s="22"/>
+      <c r="I3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <v>10</v>
+      </c>
+      <c r="B4" s="21">
+        <f>A4*J$3</f>
+        <v>1000</v>
+      </c>
+      <c r="C4" s="20">
+        <f>J$2*J$2/B4</f>
+        <v>52.9</v>
+      </c>
+      <c r="D4" s="20">
+        <f>D$3</f>
+        <v>74.06</v>
+      </c>
+      <c r="E4" s="22">
+        <f t="shared" ref="E4:E11" si="0">C4-D4</f>
+        <v>-21.160000000000004</v>
+      </c>
+      <c r="F4" s="20">
+        <f>F$3</f>
+        <v>100.13</v>
+      </c>
+      <c r="G4" s="22">
+        <f t="shared" ref="G4:G11" si="1">C4-F4</f>
+        <v>-47.23</v>
+      </c>
+      <c r="H4" s="22"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <v>5</v>
+      </c>
+      <c r="B5" s="21">
+        <f>A5*J$3</f>
+        <v>500</v>
+      </c>
+      <c r="C5" s="20">
+        <f>J$2*J$2/B5</f>
+        <v>105.8</v>
+      </c>
+      <c r="D5" s="20">
+        <f t="shared" ref="D5:F11" si="2">D$3</f>
+        <v>74.06</v>
+      </c>
+      <c r="E5" s="22">
+        <f t="shared" si="0"/>
+        <v>31.739999999999995</v>
+      </c>
+      <c r="F5" s="20">
+        <f t="shared" si="2"/>
+        <v>100.13</v>
+      </c>
+      <c r="G5" s="22">
+        <f t="shared" si="1"/>
+        <v>5.6700000000000017</v>
+      </c>
+      <c r="H5" s="22"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="21">
+        <f>A6*J$3</f>
+        <v>400</v>
+      </c>
+      <c r="C6" s="20">
+        <f>J$2*J$2/B6</f>
+        <v>132.25</v>
+      </c>
+      <c r="D6" s="20">
+        <f t="shared" si="2"/>
+        <v>74.06</v>
+      </c>
+      <c r="E6" s="22">
+        <f t="shared" si="0"/>
+        <v>58.19</v>
+      </c>
+      <c r="F6" s="20">
+        <f t="shared" si="2"/>
+        <v>100.13</v>
+      </c>
+      <c r="G6" s="22">
+        <f t="shared" si="1"/>
+        <v>32.120000000000005</v>
+      </c>
+      <c r="H6" s="22"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="23"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <v>3</v>
+      </c>
+      <c r="B7" s="21">
+        <f>A7*J$3</f>
+        <v>300</v>
+      </c>
+      <c r="C7" s="20">
+        <f>J$2*J$2/B7</f>
+        <v>176.33333333333334</v>
+      </c>
+      <c r="D7" s="20">
+        <f t="shared" si="2"/>
+        <v>74.06</v>
+      </c>
+      <c r="E7" s="22">
+        <f t="shared" si="0"/>
+        <v>102.27333333333334</v>
+      </c>
+      <c r="F7" s="20">
+        <f t="shared" si="2"/>
+        <v>100.13</v>
+      </c>
+      <c r="G7" s="22">
+        <f t="shared" si="1"/>
+        <v>76.203333333333347</v>
+      </c>
+      <c r="H7" s="22"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="B8" s="21">
+        <f>A8*J$3</f>
+        <v>250</v>
+      </c>
+      <c r="C8" s="20">
+        <f>J$2*J$2/B8</f>
+        <v>211.6</v>
+      </c>
+      <c r="D8" s="20">
+        <f t="shared" si="2"/>
+        <v>74.06</v>
+      </c>
+      <c r="E8" s="22">
+        <f t="shared" si="0"/>
+        <v>137.54</v>
+      </c>
+      <c r="F8" s="20">
+        <f t="shared" si="2"/>
+        <v>100.13</v>
+      </c>
+      <c r="G8" s="22">
+        <f t="shared" si="1"/>
+        <v>111.47</v>
+      </c>
+      <c r="H8" s="22"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="6">
+        <v>2</v>
+      </c>
+      <c r="B9" s="21">
+        <f>A9*J$3</f>
+        <v>200</v>
+      </c>
+      <c r="C9" s="20">
+        <f>J$2*J$2/B9</f>
+        <v>264.5</v>
+      </c>
+      <c r="D9" s="20">
+        <f t="shared" si="2"/>
+        <v>74.06</v>
+      </c>
+      <c r="E9" s="22">
+        <f t="shared" si="0"/>
+        <v>190.44</v>
+      </c>
+      <c r="F9" s="20">
+        <f t="shared" si="2"/>
+        <v>100.13</v>
+      </c>
+      <c r="G9" s="22">
+        <f t="shared" si="1"/>
+        <v>164.37</v>
+      </c>
+      <c r="H9" s="22"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="6">
+        <v>1.5</v>
+      </c>
+      <c r="B10" s="21">
+        <f>A10*J$3</f>
+        <v>150</v>
+      </c>
+      <c r="C10" s="20">
+        <f>J$2*J$2/B10</f>
+        <v>352.66666666666669</v>
+      </c>
+      <c r="D10" s="20">
+        <f t="shared" si="2"/>
+        <v>74.06</v>
+      </c>
+      <c r="E10" s="22">
+        <f t="shared" ref="E10" si="3">C10-D10</f>
+        <v>278.60666666666668</v>
+      </c>
+      <c r="F10" s="20">
+        <f t="shared" si="2"/>
+        <v>100.13</v>
+      </c>
+      <c r="G10" s="22">
+        <f t="shared" ref="G10" si="4">C10-F10</f>
+        <v>252.53666666666669</v>
+      </c>
+      <c r="H10" s="22"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="6">
+        <v>1</v>
+      </c>
+      <c r="B11" s="21">
+        <f>A11*J$3</f>
+        <v>100</v>
+      </c>
+      <c r="C11" s="20">
+        <f>J$2*J$2/B11</f>
+        <v>529</v>
+      </c>
+      <c r="D11" s="20">
+        <f t="shared" si="2"/>
+        <v>74.06</v>
+      </c>
+      <c r="E11" s="22">
+        <f t="shared" si="0"/>
+        <v>454.94</v>
+      </c>
+      <c r="F11" s="20">
+        <f t="shared" si="2"/>
+        <v>100.13</v>
+      </c>
+      <c r="G11" s="22">
+        <f t="shared" si="1"/>
+        <v>428.87</v>
+      </c>
+      <c r="H11" s="22"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="D12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H1">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="6">
-        <v>20</v>
-      </c>
-      <c r="B2" s="21">
-        <f>A2*H$2</f>
-        <v>2000</v>
-      </c>
-      <c r="C2" s="20">
-        <f>H$1*H$1/B2</f>
-        <v>26.45</v>
-      </c>
-      <c r="D2" s="22">
-        <f>C2-H$4</f>
-        <v>-37.03</v>
-      </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="6">
-        <v>10</v>
-      </c>
-      <c r="B3" s="21">
-        <f t="shared" ref="B3:B9" si="0">A3*H$2</f>
-        <v>1000</v>
-      </c>
-      <c r="C3" s="20">
-        <f t="shared" ref="C3:C9" si="1">H$1*H$1/B3</f>
-        <v>52.9</v>
-      </c>
-      <c r="D3" s="22">
-        <f>C3-H$4</f>
-        <v>-10.579999999999998</v>
-      </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H3">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
-        <v>5</v>
-      </c>
-      <c r="B4" s="21">
-        <f t="shared" si="0"/>
-        <v>500</v>
-      </c>
-      <c r="C4" s="20">
-        <f t="shared" si="1"/>
-        <v>105.8</v>
-      </c>
-      <c r="D4" s="22">
-        <f t="shared" ref="D4:D9" si="2">C4-H$4</f>
-        <v>42.32</v>
-      </c>
-      <c r="E4" s="22">
-        <f>D4*COS(85/57.2957)</f>
-        <v>3.6883442364681684</v>
-      </c>
-      <c r="F4" s="22">
-        <f>D4*SIN(85/57.2957)</f>
-        <v>42.158967216872284</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4">
-        <f>H1*H1*H3/H2</f>
-        <v>63.48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
-        <v>4</v>
-      </c>
-      <c r="B5" s="21">
-        <f t="shared" si="0"/>
-        <v>400</v>
-      </c>
-      <c r="C5" s="20">
-        <f t="shared" si="1"/>
-        <v>132.25</v>
-      </c>
-      <c r="D5" s="22">
-        <f t="shared" si="2"/>
-        <v>68.77000000000001</v>
-      </c>
-      <c r="E5" s="22">
-        <f t="shared" ref="E5:E9" si="3">D5*COS(85/57.2957)</f>
-        <v>5.9935593842607746</v>
-      </c>
-      <c r="F5" s="22">
-        <f t="shared" ref="F5:F9" si="4">D5*SIN(85/57.2957)</f>
-        <v>68.508321727417467</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H5" s="23">
-        <f>1/H3</f>
-        <v>8.3333333333333339</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
-        <v>3</v>
-      </c>
-      <c r="B6" s="21">
-        <f t="shared" si="0"/>
-        <v>300</v>
-      </c>
-      <c r="C6" s="20">
-        <f t="shared" si="1"/>
-        <v>176.33333333333334</v>
-      </c>
-      <c r="D6" s="22">
-        <f t="shared" si="2"/>
-        <v>112.85333333333335</v>
-      </c>
-      <c r="E6" s="22">
-        <f t="shared" si="3"/>
-        <v>9.8355846305817849</v>
-      </c>
-      <c r="F6" s="22">
-        <f t="shared" si="4"/>
-        <v>112.42391257832611</v>
-      </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
-        <v>2.5</v>
-      </c>
-      <c r="B7" s="21">
-        <f t="shared" si="0"/>
-        <v>250</v>
-      </c>
-      <c r="C7" s="20">
-        <f t="shared" si="1"/>
-        <v>211.6</v>
-      </c>
-      <c r="D7" s="22">
-        <f t="shared" si="2"/>
-        <v>148.12</v>
-      </c>
-      <c r="E7" s="22">
-        <f t="shared" si="3"/>
-        <v>12.90920482763859</v>
-      </c>
-      <c r="F7" s="22">
-        <f t="shared" si="4"/>
-        <v>147.556385259053</v>
-      </c>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
-        <v>2</v>
-      </c>
-      <c r="B8" s="21">
-        <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="C8" s="20">
-        <f t="shared" si="1"/>
-        <v>264.5</v>
-      </c>
-      <c r="D8" s="22">
-        <f t="shared" si="2"/>
-        <v>201.02</v>
-      </c>
-      <c r="E8" s="22">
-        <f t="shared" si="3"/>
-        <v>17.5196351232238</v>
-      </c>
-      <c r="F8" s="22">
-        <f t="shared" si="4"/>
-        <v>200.25509428014337</v>
-      </c>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
-        <v>1</v>
-      </c>
-      <c r="B9" s="21">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="C9" s="20">
-        <f t="shared" si="1"/>
-        <v>529</v>
-      </c>
-      <c r="D9" s="22">
-        <f t="shared" si="2"/>
-        <v>465.52</v>
-      </c>
-      <c r="E9" s="22">
-        <f t="shared" si="3"/>
-        <v>40.571786601149853</v>
-      </c>
-      <c r="F9" s="22">
-        <f t="shared" si="4"/>
-        <v>463.74863938559508</v>
-      </c>
-      <c r="G9" s="1"/>
+      <c r="E12" s="22">
+        <f>$J$2*$J$2/$D$3/100</f>
+        <v>7.1428571428571423</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="22">
+        <f>$J$2*$J$2/$F$3/100</f>
+        <v>5.283131928492959</v>
+      </c>
+      <c r="H12" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
working on SolarSystem example for PSCAD
</commit_message>
<xml_diff>
--- a/emt-bootcamp/Support/EMTBootCamp.xlsx
+++ b/emt-bootcamp/Support/EMTBootCamp.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\i2x\emt-bootcamp\Support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25267ACC-00E8-4742-ADC0-E9C373FC30C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6043CF7A-9568-4C49-BD28-11237C08EC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="3740" windowWidth="20210" windowHeight="10660" activeTab="3" xr2:uid="{A8C2E3F1-142E-440E-A762-DE7B4CF8E5D3}"/>
+    <workbookView xWindow="8460" yWindow="10580" windowWidth="21200" windowHeight="13810" activeTab="4" xr2:uid="{A8C2E3F1-142E-440E-A762-DE7B4CF8E5D3}"/>
   </bookViews>
   <sheets>
     <sheet name="COMTRADE" sheetId="1" r:id="rId1"/>
     <sheet name="Source" sheetId="2" r:id="rId2"/>
     <sheet name="Weak" sheetId="3" r:id="rId3"/>
     <sheet name="StepSCR" sheetId="4" r:id="rId4"/>
+    <sheet name="IEEE39m" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Dmax">COMTRADE!$N$2</definedName>
@@ -24,15 +25,20 @@
     <definedName name="Ibase">COMTRADE!$N$5</definedName>
     <definedName name="IpuMax">COMTRADE!$N$10</definedName>
     <definedName name="Iscale">COMTRADE!$N$7</definedName>
+    <definedName name="kvb">IEEE39m!$AF$1</definedName>
+    <definedName name="mips">IEEE39m!$AJ$1</definedName>
+    <definedName name="sb">IEEE39m!$AG$1</definedName>
     <definedName name="Splant">COMTRADE!$N$3</definedName>
     <definedName name="SpuMax">COMTRADE!$N$11</definedName>
     <definedName name="Sscale">COMTRADE!$N$8</definedName>
     <definedName name="Vpoc">COMTRADE!$N$4</definedName>
     <definedName name="VpuMax">COMTRADE!$N$9</definedName>
     <definedName name="Vscale">COMTRADE!$N$6</definedName>
+    <definedName name="wb">IEEE39m!$AH$1</definedName>
     <definedName name="XS" localSheetId="3">StepSCR!$J$6</definedName>
     <definedName name="XS" localSheetId="2">Weak!$F$5</definedName>
     <definedName name="XS">Source!$F$5</definedName>
+    <definedName name="zb">IEEE39m!$AI$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="97">
   <si>
     <t>Name</t>
   </si>
@@ -323,6 +329,111 @@
   <si>
     <t>SCR Xplant</t>
   </si>
+  <si>
+    <t>Gen</t>
+  </si>
+  <si>
+    <t>Bus</t>
+  </si>
+  <si>
+    <t>Pg</t>
+  </si>
+  <si>
+    <t>Qg</t>
+  </si>
+  <si>
+    <t>Vg</t>
+  </si>
+  <si>
+    <t>Pmax</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>PSCAD</t>
+  </si>
+  <si>
+    <t>EMTP</t>
+  </si>
+  <si>
+    <t>inf bus</t>
+  </si>
+  <si>
+    <t>Pd</t>
+  </si>
+  <si>
+    <t>Qd</t>
+  </si>
+  <si>
+    <t>Matpower Buses</t>
+  </si>
+  <si>
+    <t>Matpower Branches</t>
+  </si>
+  <si>
+    <t>Vm</t>
+  </si>
+  <si>
+    <t>Va</t>
+  </si>
+  <si>
+    <t>kVbase</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>S (normal)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Zsurge</t>
+  </si>
+  <si>
+    <t>V [us]</t>
+  </si>
+  <si>
+    <t>Len [mi]</t>
+  </si>
+  <si>
+    <t>Loads</t>
+  </si>
+  <si>
+    <t>Total Gen</t>
+  </si>
+  <si>
+    <t>Losses</t>
+  </si>
+  <si>
+    <t>Matpower Dispatch</t>
+  </si>
 </sst>
 </file>
 
@@ -335,7 +446,7 @@
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,6 +469,33 @@
       <name val="Symbol"/>
       <family val="1"/>
       <charset val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000080"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF303080"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="3">
@@ -386,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -445,6 +583,55 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -766,7 +953,7 @@
       <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="4" max="4" width="8.7265625" customWidth="1"/>
     <col min="5" max="5" width="7.6328125" customWidth="1"/>
@@ -778,7 +965,7 @@
     <col min="13" max="13" width="9.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="29">
       <c r="A1" s="14" t="s">
         <v>43</v>
       </c>
@@ -819,7 +1006,7 @@
         <v>-32767</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -864,7 +1051,7 @@
         <v>32767</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -909,7 +1096,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -954,7 +1141,7 @@
         <v>230000</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1000,7 +1187,7 @@
         <v>251.02185616940253</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1045,7 +1232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1090,7 +1277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1134,7 +1321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1179,7 +1366,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1224,7 +1411,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1281,13 +1468,13 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
@@ -1304,7 +1491,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6">
       <c r="A2" s="6">
         <v>0.01</v>
       </c>
@@ -1323,7 +1510,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6">
       <c r="A3" s="6">
         <v>0.25</v>
       </c>
@@ -1343,7 +1530,7 @@
         <v>1.4835298641951802</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6">
       <c r="A4" s="6">
         <v>0.5</v>
       </c>
@@ -1363,7 +1550,7 @@
         <v>0.87155742747658138</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6">
       <c r="A5" s="6">
         <v>0.8</v>
       </c>
@@ -1383,7 +1570,7 @@
         <v>9.961946980917455</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6">
       <c r="E6" s="1" t="s">
         <v>54</v>
       </c>
@@ -1391,7 +1578,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6">
       <c r="E7" s="1" t="s">
         <v>51</v>
       </c>
@@ -1400,7 +1587,7 @@
         <v>5290</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6">
       <c r="E8" s="1" t="s">
         <v>52</v>
       </c>
@@ -1408,7 +1595,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6">
       <c r="E9" s="1" t="s">
         <v>53</v>
       </c>
@@ -1431,13 +1618,13 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>37</v>
       </c>
@@ -1454,7 +1641,7 @@
         <v>211.6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6">
       <c r="A2" s="6">
         <v>0.01</v>
       </c>
@@ -1473,7 +1660,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6">
       <c r="A3" s="6">
         <v>0.25</v>
       </c>
@@ -1493,7 +1680,7 @@
         <v>1.4835298641951802</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6">
       <c r="A4" s="6">
         <v>0.5</v>
       </c>
@@ -1513,7 +1700,7 @@
         <v>18.442155165404461</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6">
       <c r="A5" s="6">
         <v>0.8</v>
       </c>
@@ -1533,7 +1720,7 @@
         <v>210.79479811621334</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6">
       <c r="E6" s="1" t="s">
         <v>54</v>
       </c>
@@ -1541,7 +1728,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6">
       <c r="E7" s="1" t="s">
         <v>51</v>
       </c>
@@ -1550,7 +1737,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6">
       <c r="E8" s="1" t="s">
         <v>52</v>
       </c>
@@ -1558,7 +1745,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6">
       <c r="E9" s="1" t="s">
         <v>53</v>
       </c>
@@ -1577,18 +1764,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70A51ED4-A577-4B06-8042-A04C86E2D43B}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.36328125" customWidth="1"/>
     <col min="5" max="8" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10">
       <c r="D1" s="1" t="s">
         <v>60</v>
       </c>
@@ -1596,7 +1783,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10">
       <c r="A2" s="4" t="s">
         <v>53</v>
       </c>
@@ -1626,16 +1813,16 @@
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10">
       <c r="A3" s="6">
         <v>20</v>
       </c>
       <c r="B3" s="21">
-        <f>A3*J$3</f>
+        <f t="shared" ref="B3:B11" si="0">A3*J$3</f>
         <v>2000</v>
       </c>
       <c r="C3" s="20">
-        <f>J$2*J$2/B3</f>
+        <f t="shared" ref="C3:C11" si="1">J$2*J$2/B3</f>
         <v>26.45</v>
       </c>
       <c r="D3" s="24">
@@ -1660,16 +1847,16 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10">
       <c r="A4" s="6">
         <v>10</v>
       </c>
       <c r="B4" s="21">
-        <f>A4*J$3</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="C4" s="20">
-        <f>J$2*J$2/B4</f>
+        <f t="shared" si="1"/>
         <v>52.9</v>
       </c>
       <c r="D4" s="20">
@@ -1677,7 +1864,7 @@
         <v>74.06</v>
       </c>
       <c r="E4" s="22">
-        <f t="shared" ref="E4:E11" si="0">C4-D4</f>
+        <f t="shared" ref="E4:E11" si="2">C4-D4</f>
         <v>-21.160000000000004</v>
       </c>
       <c r="F4" s="20">
@@ -1685,231 +1872,231 @@
         <v>100.13</v>
       </c>
       <c r="G4" s="22">
-        <f t="shared" ref="G4:G11" si="1">C4-F4</f>
+        <f t="shared" ref="G4:G11" si="3">C4-F4</f>
         <v>-47.23</v>
       </c>
       <c r="H4" s="22"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10">
       <c r="A5" s="6">
         <v>5</v>
       </c>
       <c r="B5" s="21">
-        <f>A5*J$3</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="C5" s="20">
-        <f>J$2*J$2/B5</f>
+        <f t="shared" si="1"/>
         <v>105.8</v>
       </c>
       <c r="D5" s="20">
-        <f t="shared" ref="D5:F11" si="2">D$3</f>
+        <f t="shared" ref="D5:F11" si="4">D$3</f>
         <v>74.06</v>
       </c>
       <c r="E5" s="22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>31.739999999999995</v>
       </c>
       <c r="F5" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100.13</v>
       </c>
       <c r="G5" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.6700000000000017</v>
       </c>
       <c r="H5" s="22"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10">
       <c r="A6" s="6">
         <v>4</v>
       </c>
       <c r="B6" s="21">
-        <f>A6*J$3</f>
+        <f t="shared" si="0"/>
         <v>400</v>
       </c>
       <c r="C6" s="20">
-        <f>J$2*J$2/B6</f>
+        <f t="shared" si="1"/>
         <v>132.25</v>
       </c>
       <c r="D6" s="20">
+        <f t="shared" si="4"/>
+        <v>74.06</v>
+      </c>
+      <c r="E6" s="22">
         <f t="shared" si="2"/>
-        <v>74.06</v>
-      </c>
-      <c r="E6" s="22">
-        <f t="shared" si="0"/>
         <v>58.19</v>
       </c>
       <c r="F6" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100.13</v>
       </c>
       <c r="G6" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>32.120000000000005</v>
       </c>
       <c r="H6" s="22"/>
       <c r="I6" s="1"/>
       <c r="J6" s="23"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10">
       <c r="A7" s="6">
         <v>3</v>
       </c>
       <c r="B7" s="21">
-        <f>A7*J$3</f>
+        <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="C7" s="20">
-        <f>J$2*J$2/B7</f>
+        <f t="shared" si="1"/>
         <v>176.33333333333334</v>
       </c>
       <c r="D7" s="20">
+        <f t="shared" si="4"/>
+        <v>74.06</v>
+      </c>
+      <c r="E7" s="22">
         <f t="shared" si="2"/>
-        <v>74.06</v>
-      </c>
-      <c r="E7" s="22">
-        <f t="shared" si="0"/>
         <v>102.27333333333334</v>
       </c>
       <c r="F7" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100.13</v>
       </c>
       <c r="G7" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>76.203333333333347</v>
       </c>
       <c r="H7" s="22"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10">
       <c r="A8" s="6">
         <v>2.5</v>
       </c>
       <c r="B8" s="21">
-        <f>A8*J$3</f>
+        <f t="shared" si="0"/>
         <v>250</v>
       </c>
       <c r="C8" s="20">
-        <f>J$2*J$2/B8</f>
+        <f t="shared" si="1"/>
         <v>211.6</v>
       </c>
       <c r="D8" s="20">
+        <f t="shared" si="4"/>
+        <v>74.06</v>
+      </c>
+      <c r="E8" s="22">
         <f t="shared" si="2"/>
-        <v>74.06</v>
-      </c>
-      <c r="E8" s="22">
-        <f t="shared" si="0"/>
         <v>137.54</v>
       </c>
       <c r="F8" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100.13</v>
       </c>
       <c r="G8" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>111.47</v>
       </c>
       <c r="H8" s="22"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10">
       <c r="A9" s="6">
         <v>2</v>
       </c>
       <c r="B9" s="21">
-        <f>A9*J$3</f>
+        <f t="shared" si="0"/>
         <v>200</v>
       </c>
       <c r="C9" s="20">
-        <f>J$2*J$2/B9</f>
+        <f t="shared" si="1"/>
         <v>264.5</v>
       </c>
       <c r="D9" s="20">
+        <f t="shared" si="4"/>
+        <v>74.06</v>
+      </c>
+      <c r="E9" s="22">
         <f t="shared" si="2"/>
-        <v>74.06</v>
-      </c>
-      <c r="E9" s="22">
-        <f t="shared" si="0"/>
         <v>190.44</v>
       </c>
       <c r="F9" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100.13</v>
       </c>
       <c r="G9" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>164.37</v>
       </c>
       <c r="H9" s="22"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10">
       <c r="A10" s="6">
         <v>1.5</v>
       </c>
       <c r="B10" s="21">
-        <f>A10*J$3</f>
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="C10" s="20">
-        <f>J$2*J$2/B10</f>
+        <f t="shared" si="1"/>
         <v>352.66666666666669</v>
       </c>
       <c r="D10" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>74.06</v>
       </c>
       <c r="E10" s="22">
-        <f t="shared" ref="E10" si="3">C10-D10</f>
+        <f t="shared" ref="E10" si="5">C10-D10</f>
         <v>278.60666666666668</v>
       </c>
       <c r="F10" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100.13</v>
       </c>
       <c r="G10" s="22">
-        <f t="shared" ref="G10" si="4">C10-F10</f>
+        <f t="shared" ref="G10" si="6">C10-F10</f>
         <v>252.53666666666669</v>
       </c>
       <c r="H10" s="22"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10">
       <c r="A11" s="6">
         <v>1</v>
       </c>
       <c r="B11" s="21">
-        <f>A11*J$3</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="C11" s="20">
-        <f>J$2*J$2/B11</f>
+        <f t="shared" si="1"/>
         <v>529</v>
       </c>
       <c r="D11" s="20">
+        <f t="shared" si="4"/>
+        <v>74.06</v>
+      </c>
+      <c r="E11" s="22">
         <f t="shared" si="2"/>
-        <v>74.06</v>
-      </c>
-      <c r="E11" s="22">
-        <f t="shared" si="0"/>
         <v>454.94</v>
       </c>
       <c r="F11" s="20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>100.13</v>
       </c>
       <c r="G11" s="22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>428.87</v>
       </c>
       <c r="H11" s="22"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10">
       <c r="D12" s="1" t="s">
         <v>61</v>
       </c>
@@ -1930,4 +2117,3349 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F98AF1C0-18B6-49C9-8A8E-53F5401F1E81}">
+  <dimension ref="A1:AJ48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N19" sqref="N19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="6" width="8.7265625" style="5"/>
+    <col min="7" max="7" width="3.7265625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="3.54296875" customWidth="1"/>
+    <col min="15" max="15" width="4.7265625" customWidth="1"/>
+    <col min="19" max="19" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.08984375" customWidth="1"/>
+    <col min="23" max="23" width="6.81640625" customWidth="1"/>
+    <col min="24" max="24" width="7.36328125" customWidth="1"/>
+    <col min="25" max="25" width="6.6328125" customWidth="1"/>
+    <col min="26" max="26" width="11.1796875" customWidth="1"/>
+    <col min="31" max="31" width="4.08984375" customWidth="1"/>
+    <col min="33" max="33" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36">
+      <c r="A1" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="P1" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="W1" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="35"/>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="36">
+        <v>345</v>
+      </c>
+      <c r="AG1" s="1">
+        <v>100</v>
+      </c>
+      <c r="AH1" s="1">
+        <f>60*2*PI()</f>
+        <v>376.99111843077515</v>
+      </c>
+      <c r="AI1" s="1">
+        <f>kvb*kvb/sb</f>
+        <v>1190.25</v>
+      </c>
+      <c r="AJ1" s="39">
+        <v>180000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36">
+      <c r="A2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AG2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="AH2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI2" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AJ2" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="28">
+        <v>30</v>
+      </c>
+      <c r="C3" s="28">
+        <v>250</v>
+      </c>
+      <c r="D3" s="29">
+        <v>161.762</v>
+      </c>
+      <c r="E3" s="30">
+        <v>1.0499000000000001</v>
+      </c>
+      <c r="F3" s="28">
+        <v>1040</v>
+      </c>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28">
+        <v>250</v>
+      </c>
+      <c r="I3" s="28">
+        <v>1.048</v>
+      </c>
+      <c r="J3">
+        <v>800</v>
+      </c>
+      <c r="L3">
+        <v>250</v>
+      </c>
+      <c r="M3">
+        <f>20.9/20</f>
+        <v>1.0449999999999999</v>
+      </c>
+      <c r="N3">
+        <v>1000</v>
+      </c>
+      <c r="P3" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="27">
+        <v>97.6</v>
+      </c>
+      <c r="R3" s="27">
+        <v>44.2</v>
+      </c>
+      <c r="S3" s="37">
+        <v>1.0393836000000001</v>
+      </c>
+      <c r="T3" s="38">
+        <v>-13.536602</v>
+      </c>
+      <c r="U3" s="25">
+        <v>345</v>
+      </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
+      <c r="X3" s="25">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="25">
+        <v>2</v>
+      </c>
+      <c r="Z3" s="27">
+        <v>600</v>
+      </c>
+      <c r="AA3" s="26">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="AB3" s="26">
+        <v>4.1099999999999998E-2</v>
+      </c>
+      <c r="AC3" s="26">
+        <v>0.69869999999999999</v>
+      </c>
+      <c r="AD3" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="27"/>
+      <c r="AF3">
+        <f>AB3*zb/wb</f>
+        <v>0.129762407145363</v>
+      </c>
+      <c r="AG3">
+        <f>AC3*sb/wb/kvb/kvb</f>
+        <v>1.557117674694494E-6</v>
+      </c>
+      <c r="AH3">
+        <f>SQRT(AF3/AG3)</f>
+        <v>288.67802769949532</v>
+      </c>
+      <c r="AI3" s="23">
+        <f>1000000*SQRT(AF3*AG3)</f>
+        <v>449.50565922683091</v>
+      </c>
+      <c r="AJ3" s="23">
+        <f>0.000001*AI3*mips</f>
+        <v>80.911018660829555</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36">
+      <c r="A4" s="31">
+        <v>2</v>
+      </c>
+      <c r="B4" s="32">
+        <v>31</v>
+      </c>
+      <c r="C4" s="33">
+        <v>677.87099999999998</v>
+      </c>
+      <c r="D4" s="34">
+        <v>221.57400000000001</v>
+      </c>
+      <c r="E4" s="33">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="F4" s="34">
+        <v>646</v>
+      </c>
+      <c r="G4" s="42"/>
+      <c r="H4" s="43">
+        <v>547.32600000000002</v>
+      </c>
+      <c r="I4" s="42">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="J4">
+        <v>800</v>
+      </c>
+      <c r="L4" s="40">
+        <v>572.16</v>
+      </c>
+      <c r="M4">
+        <f>19.6/20</f>
+        <v>0.98000000000000009</v>
+      </c>
+      <c r="N4">
+        <v>1000</v>
+      </c>
+      <c r="P4" s="25">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="27">
+        <v>0</v>
+      </c>
+      <c r="R4" s="27">
+        <v>0</v>
+      </c>
+      <c r="S4" s="37">
+        <v>1.0484941000000001</v>
+      </c>
+      <c r="T4" s="38">
+        <v>-9.7852665999999999</v>
+      </c>
+      <c r="U4" s="25">
+        <v>345</v>
+      </c>
+      <c r="W4">
+        <v>2</v>
+      </c>
+      <c r="X4" s="25">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="25">
+        <v>39</v>
+      </c>
+      <c r="Z4" s="25">
+        <v>1000</v>
+      </c>
+      <c r="AA4" s="26">
+        <v>1E-3</v>
+      </c>
+      <c r="AB4" s="26">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AC4" s="26">
+        <v>0.75</v>
+      </c>
+      <c r="AD4" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="27"/>
+      <c r="AF4">
+        <f>AB4*zb/wb</f>
+        <v>7.8930904589636849E-2</v>
+      </c>
+      <c r="AG4">
+        <f>AC4*sb/wb/kvb/kvb</f>
+        <v>1.6714444769155149E-6</v>
+      </c>
+      <c r="AH4">
+        <f t="shared" ref="AH4:AH6" si="0">SQRT(AF4/AG4)</f>
+        <v>217.30892469017468</v>
+      </c>
+      <c r="AI4" s="23">
+        <f t="shared" ref="AI4:AI6" si="1">1000000*SQRT(AF4*AG4)</f>
+        <v>363.21980195784198</v>
+      </c>
+      <c r="AJ4" s="23">
+        <f>0.000001*AI4*mips</f>
+        <v>65.379564352411549</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="28">
+        <v>32</v>
+      </c>
+      <c r="C5" s="28">
+        <v>650</v>
+      </c>
+      <c r="D5" s="29">
+        <v>206.965</v>
+      </c>
+      <c r="E5" s="30">
+        <v>0.98409999999999997</v>
+      </c>
+      <c r="F5" s="29">
+        <v>725</v>
+      </c>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29">
+        <v>650</v>
+      </c>
+      <c r="I5" s="29">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="J5">
+        <v>800</v>
+      </c>
+      <c r="L5">
+        <v>650</v>
+      </c>
+      <c r="M5">
+        <f>19.662/20</f>
+        <v>0.98309999999999997</v>
+      </c>
+      <c r="N5">
+        <v>1000</v>
+      </c>
+      <c r="P5" s="25">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="27">
+        <v>322</v>
+      </c>
+      <c r="R5" s="27">
+        <v>2.4</v>
+      </c>
+      <c r="S5" s="37">
+        <v>1.0307077</v>
+      </c>
+      <c r="T5" s="38">
+        <v>-12.276384</v>
+      </c>
+      <c r="U5" s="25">
+        <v>345</v>
+      </c>
+      <c r="W5">
+        <v>3</v>
+      </c>
+      <c r="X5" s="25">
+        <v>2</v>
+      </c>
+      <c r="Y5" s="25">
+        <v>3</v>
+      </c>
+      <c r="Z5" s="27">
+        <v>500</v>
+      </c>
+      <c r="AA5" s="26">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="AB5" s="26">
+        <v>1.5100000000000001E-2</v>
+      </c>
+      <c r="AC5" s="26">
+        <v>0.25719999999999998</v>
+      </c>
+      <c r="AD5" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="27"/>
+      <c r="AF5">
+        <f>AB5*zb/wb</f>
+        <v>4.7674266372140665E-2</v>
+      </c>
+      <c r="AG5">
+        <f>AC5*sb/wb/kvb/kvb</f>
+        <v>5.7319402595022729E-7</v>
+      </c>
+      <c r="AH5">
+        <f t="shared" si="0"/>
+        <v>288.39729435710058</v>
+      </c>
+      <c r="AI5" s="23">
+        <f t="shared" si="1"/>
+        <v>165.30760622569926</v>
+      </c>
+      <c r="AJ5" s="23">
+        <f>0.000001*AI5*mips</f>
+        <v>29.755369120625868</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6" s="28">
+        <v>33</v>
+      </c>
+      <c r="C6" s="28">
+        <v>632</v>
+      </c>
+      <c r="D6" s="29">
+        <v>108.29300000000001</v>
+      </c>
+      <c r="E6" s="30">
+        <v>0.99719999999999998</v>
+      </c>
+      <c r="F6" s="29">
+        <v>652</v>
+      </c>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29">
+        <v>632</v>
+      </c>
+      <c r="I6" s="29">
+        <v>0.997</v>
+      </c>
+      <c r="J6">
+        <v>800</v>
+      </c>
+      <c r="L6">
+        <v>632</v>
+      </c>
+      <c r="M6">
+        <f>19.944/20</f>
+        <v>0.99719999999999998</v>
+      </c>
+      <c r="N6">
+        <v>1000</v>
+      </c>
+      <c r="P6" s="25">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="27">
+        <v>500</v>
+      </c>
+      <c r="R6" s="27">
+        <v>184</v>
+      </c>
+      <c r="S6" s="37">
+        <v>1.0044599999999999</v>
+      </c>
+      <c r="T6" s="38">
+        <v>-12.626734000000001</v>
+      </c>
+      <c r="U6" s="25">
+        <v>345</v>
+      </c>
+      <c r="W6">
+        <v>4</v>
+      </c>
+      <c r="X6" s="25">
+        <v>2</v>
+      </c>
+      <c r="Y6" s="25">
+        <v>25</v>
+      </c>
+      <c r="Z6" s="27">
+        <v>500</v>
+      </c>
+      <c r="AA6" s="26">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AB6" s="26">
+        <v>8.6E-3</v>
+      </c>
+      <c r="AC6" s="26">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="AD6" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="27"/>
+      <c r="AF6">
+        <f>AB6*zb/wb</f>
+        <v>2.7152231178835078E-2</v>
+      </c>
+      <c r="AG6">
+        <f>AC6*sb/wb/kvb/kvb</f>
+        <v>3.253745248395536E-7</v>
+      </c>
+      <c r="AH6">
+        <f t="shared" si="0"/>
+        <v>288.87568470841126</v>
+      </c>
+      <c r="AI6" s="23">
+        <f t="shared" si="1"/>
+        <v>93.992788649700017</v>
+      </c>
+      <c r="AJ6" s="23">
+        <f>0.000001*AI6*mips</f>
+        <v>16.918701956946002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36">
+      <c r="A7" s="5">
+        <v>5</v>
+      </c>
+      <c r="B7" s="28">
+        <v>34</v>
+      </c>
+      <c r="C7" s="28">
+        <v>508</v>
+      </c>
+      <c r="D7" s="29">
+        <v>166.68799999999999</v>
+      </c>
+      <c r="E7" s="30">
+        <v>1.0123</v>
+      </c>
+      <c r="F7" s="29">
+        <v>508</v>
+      </c>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29">
+        <v>508</v>
+      </c>
+      <c r="I7" s="29">
+        <v>1.012</v>
+      </c>
+      <c r="J7">
+        <v>800</v>
+      </c>
+      <c r="L7">
+        <v>508</v>
+      </c>
+      <c r="M7" s="40">
+        <f>20.15/20</f>
+        <v>1.0074999999999998</v>
+      </c>
+      <c r="N7">
+        <v>600</v>
+      </c>
+      <c r="P7" s="25">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="27">
+        <v>0</v>
+      </c>
+      <c r="R7" s="27">
+        <v>0</v>
+      </c>
+      <c r="S7" s="37">
+        <v>1.0060062999999999</v>
+      </c>
+      <c r="T7" s="38">
+        <v>-11.192339</v>
+      </c>
+      <c r="U7" s="25">
+        <v>345</v>
+      </c>
+      <c r="W7">
+        <v>5</v>
+      </c>
+      <c r="X7" s="25">
+        <v>2</v>
+      </c>
+      <c r="Y7" s="25">
+        <v>30</v>
+      </c>
+      <c r="Z7" s="27">
+        <v>900</v>
+      </c>
+      <c r="AA7" s="25">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="26">
+        <v>1.8100000000000002E-2</v>
+      </c>
+      <c r="AC7" s="25">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="26">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="AE7" s="26"/>
+      <c r="AF7">
+        <f>AB7*zb/wb</f>
+        <v>5.7145974922897087E-2</v>
+      </c>
+      <c r="AG7" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36">
+      <c r="A8" s="5">
+        <v>6</v>
+      </c>
+      <c r="B8" s="28">
+        <v>35</v>
+      </c>
+      <c r="C8" s="28">
+        <v>650</v>
+      </c>
+      <c r="D8" s="29">
+        <v>210.661</v>
+      </c>
+      <c r="E8" s="30">
+        <v>1.0494000000000001</v>
+      </c>
+      <c r="F8" s="29">
+        <v>687</v>
+      </c>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29">
+        <v>650</v>
+      </c>
+      <c r="I8" s="29">
+        <v>1.0489999999999999</v>
+      </c>
+      <c r="J8">
+        <v>1000</v>
+      </c>
+      <c r="L8">
+        <v>650</v>
+      </c>
+      <c r="M8">
+        <f>20.986/20</f>
+        <v>1.0493000000000001</v>
+      </c>
+      <c r="N8">
+        <v>1000</v>
+      </c>
+      <c r="P8" s="25">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="27">
+        <v>0</v>
+      </c>
+      <c r="R8" s="27">
+        <v>0</v>
+      </c>
+      <c r="S8" s="37">
+        <v>1.0082256000000001</v>
+      </c>
+      <c r="T8" s="38">
+        <v>-10.408329999999999</v>
+      </c>
+      <c r="U8" s="25">
+        <v>345</v>
+      </c>
+      <c r="W8">
+        <v>6</v>
+      </c>
+      <c r="X8" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y8" s="25">
+        <v>4</v>
+      </c>
+      <c r="Z8" s="27">
+        <v>500</v>
+      </c>
+      <c r="AA8" s="26">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="AB8" s="26">
+        <v>2.1299999999999999E-2</v>
+      </c>
+      <c r="AC8" s="26">
+        <v>0.22140000000000001</v>
+      </c>
+      <c r="AD8" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="27"/>
+      <c r="AF8">
+        <f>AB8*zb/wb</f>
+        <v>6.72491307103706E-2</v>
+      </c>
+      <c r="AG8">
+        <f>AC8*sb/wb/kvb/kvb</f>
+        <v>4.9341040958546004E-7</v>
+      </c>
+      <c r="AH8">
+        <f t="shared" ref="AH8:AH15" si="2">SQRT(AF8/AG8)</f>
+        <v>369.18086547507693</v>
+      </c>
+      <c r="AI8" s="23">
+        <f t="shared" ref="AI8:AI15" si="3">1000000*SQRT(AF8*AG8)</f>
+        <v>182.15768204517232</v>
+      </c>
+      <c r="AJ8" s="23">
+        <f>0.000001*AI8*mips</f>
+        <v>32.788382768131015</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36">
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9" s="28">
+        <v>36</v>
+      </c>
+      <c r="C9" s="28">
+        <v>560</v>
+      </c>
+      <c r="D9" s="29">
+        <v>100.16500000000001</v>
+      </c>
+      <c r="E9" s="30">
+        <v>1.0636000000000001</v>
+      </c>
+      <c r="F9" s="29">
+        <v>580</v>
+      </c>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29">
+        <v>560</v>
+      </c>
+      <c r="I9" s="29">
+        <v>1.0640000000000001</v>
+      </c>
+      <c r="J9">
+        <v>800</v>
+      </c>
+      <c r="L9">
+        <v>560</v>
+      </c>
+      <c r="M9">
+        <f>21.27/20</f>
+        <v>1.0634999999999999</v>
+      </c>
+      <c r="N9">
+        <v>1000</v>
+      </c>
+      <c r="P9" s="25">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="26">
+        <v>233.8</v>
+      </c>
+      <c r="R9" s="27">
+        <v>84</v>
+      </c>
+      <c r="S9" s="37">
+        <v>0.99839728000000005</v>
+      </c>
+      <c r="T9" s="38">
+        <v>-12.755625999999999</v>
+      </c>
+      <c r="U9" s="25">
+        <v>345</v>
+      </c>
+      <c r="W9">
+        <v>7</v>
+      </c>
+      <c r="X9" s="25">
+        <v>3</v>
+      </c>
+      <c r="Y9" s="25">
+        <v>18</v>
+      </c>
+      <c r="Z9" s="27">
+        <v>500</v>
+      </c>
+      <c r="AA9" s="26">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="AB9" s="26">
+        <v>1.3299999999999999E-2</v>
+      </c>
+      <c r="AC9" s="26">
+        <v>0.21379999999999999</v>
+      </c>
+      <c r="AD9" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="27"/>
+      <c r="AF9">
+        <f>AB9*zb/wb</f>
+        <v>4.1991241241686801E-2</v>
+      </c>
+      <c r="AG9">
+        <f>AC9*sb/wb/kvb/kvb</f>
+        <v>4.7647310555271623E-7</v>
+      </c>
+      <c r="AH9">
+        <f t="shared" si="2"/>
+        <v>296.86579452519265</v>
+      </c>
+      <c r="AI9" s="23">
+        <f t="shared" si="3"/>
+        <v>141.44856704979307</v>
+      </c>
+      <c r="AJ9" s="23">
+        <f>0.000001*AI9*mips</f>
+        <v>25.460742068962752</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36">
+      <c r="A10" s="5">
+        <v>8</v>
+      </c>
+      <c r="B10" s="28">
+        <v>37</v>
+      </c>
+      <c r="C10" s="28">
+        <v>540</v>
+      </c>
+      <c r="D10" s="29">
+        <v>-1.3694500000000001</v>
+      </c>
+      <c r="E10" s="30">
+        <v>1.0275000000000001</v>
+      </c>
+      <c r="F10" s="29">
+        <v>564</v>
+      </c>
+      <c r="G10" s="29"/>
+      <c r="H10">
+        <v>540</v>
+      </c>
+      <c r="I10">
+        <v>1.028</v>
+      </c>
+      <c r="J10">
+        <v>800</v>
+      </c>
+      <c r="L10">
+        <v>540</v>
+      </c>
+      <c r="M10">
+        <f>20.556/20</f>
+        <v>1.0278</v>
+      </c>
+      <c r="N10">
+        <v>1000</v>
+      </c>
+      <c r="P10" s="25">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="27">
+        <v>522</v>
+      </c>
+      <c r="R10" s="26">
+        <v>176.6</v>
+      </c>
+      <c r="S10" s="37">
+        <v>0.99787232000000003</v>
+      </c>
+      <c r="T10" s="38">
+        <v>-13.335844</v>
+      </c>
+      <c r="U10" s="25">
+        <v>345</v>
+      </c>
+      <c r="W10">
+        <v>8</v>
+      </c>
+      <c r="X10" s="25">
+        <v>4</v>
+      </c>
+      <c r="Y10" s="25">
+        <v>5</v>
+      </c>
+      <c r="Z10" s="27">
+        <v>600</v>
+      </c>
+      <c r="AA10" s="26">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="AB10" s="26">
+        <v>1.2800000000000001E-2</v>
+      </c>
+      <c r="AC10" s="26">
+        <v>0.13420000000000001</v>
+      </c>
+      <c r="AD10" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="27"/>
+      <c r="AF10">
+        <f>AB10*zb/wb</f>
+        <v>4.0412623149894071E-2</v>
+      </c>
+      <c r="AG10">
+        <f>AC10*sb/wb/kvb/kvb</f>
+        <v>2.9907713173608288E-7</v>
+      </c>
+      <c r="AH10">
+        <f t="shared" si="2"/>
+        <v>367.5927329091673</v>
+      </c>
+      <c r="AI10" s="23">
+        <f t="shared" si="3"/>
+        <v>109.93858020550175</v>
+      </c>
+      <c r="AJ10" s="23">
+        <f>0.000001*AI10*mips</f>
+        <v>19.788944436990313</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36">
+      <c r="A11" s="5">
+        <v>9</v>
+      </c>
+      <c r="B11" s="28">
+        <v>38</v>
+      </c>
+      <c r="C11" s="28">
+        <v>830</v>
+      </c>
+      <c r="D11" s="29">
+        <v>21.732700000000001</v>
+      </c>
+      <c r="E11" s="30">
+        <v>1.0265</v>
+      </c>
+      <c r="F11" s="29">
+        <v>865</v>
+      </c>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29">
+        <v>830</v>
+      </c>
+      <c r="I11" s="29">
+        <v>1.0269999999999999</v>
+      </c>
+      <c r="J11">
+        <v>1000</v>
+      </c>
+      <c r="L11">
+        <v>830</v>
+      </c>
+      <c r="M11">
+        <f>20.53/20</f>
+        <v>1.0265</v>
+      </c>
+      <c r="N11">
+        <v>1000</v>
+      </c>
+      <c r="P11" s="25">
+        <v>9</v>
+      </c>
+      <c r="Q11" s="27">
+        <v>6.5</v>
+      </c>
+      <c r="R11" s="27">
+        <v>-66.599999999999994</v>
+      </c>
+      <c r="S11" s="37">
+        <v>1.038332</v>
+      </c>
+      <c r="T11" s="38">
+        <v>-14.178442</v>
+      </c>
+      <c r="U11" s="25">
+        <v>345</v>
+      </c>
+      <c r="W11">
+        <v>9</v>
+      </c>
+      <c r="X11" s="25">
+        <v>4</v>
+      </c>
+      <c r="Y11" s="25">
+        <v>14</v>
+      </c>
+      <c r="Z11" s="27">
+        <v>500</v>
+      </c>
+      <c r="AA11" s="26">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="AB11" s="26">
+        <v>1.29E-2</v>
+      </c>
+      <c r="AC11" s="26">
+        <v>0.13819999999999999</v>
+      </c>
+      <c r="AD11" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="27"/>
+      <c r="AF11">
+        <f>AB11*zb/wb</f>
+        <v>4.0728346768252613E-2</v>
+      </c>
+      <c r="AG11">
+        <f>AC11*sb/wb/kvb/kvb</f>
+        <v>3.0799150227963219E-7</v>
+      </c>
+      <c r="AH11">
+        <f t="shared" si="2"/>
+        <v>363.64617496435795</v>
+      </c>
+      <c r="AI11" s="23">
+        <f t="shared" si="3"/>
+        <v>111.99993172551457</v>
+      </c>
+      <c r="AJ11" s="23">
+        <f>0.000001*AI11*mips</f>
+        <v>20.159987710592624</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36">
+      <c r="A12" s="5">
+        <v>10</v>
+      </c>
+      <c r="B12" s="28">
+        <v>39</v>
+      </c>
+      <c r="C12" s="28">
+        <v>1000</v>
+      </c>
+      <c r="D12" s="29">
+        <v>78.467399999999998</v>
+      </c>
+      <c r="E12" s="30">
+        <v>1.03</v>
+      </c>
+      <c r="F12" s="28">
+        <v>1100</v>
+      </c>
+      <c r="G12" s="28"/>
+      <c r="H12" s="29">
+        <v>1003</v>
+      </c>
+      <c r="I12">
+        <v>1.03</v>
+      </c>
+      <c r="J12" t="s">
+        <v>71</v>
+      </c>
+      <c r="L12">
+        <v>1000</v>
+      </c>
+      <c r="M12">
+        <f>355.35/345</f>
+        <v>1.03</v>
+      </c>
+      <c r="N12">
+        <v>10000</v>
+      </c>
+      <c r="P12" s="25">
+        <v>10</v>
+      </c>
+      <c r="Q12" s="27">
+        <v>0</v>
+      </c>
+      <c r="R12" s="27">
+        <v>0</v>
+      </c>
+      <c r="S12" s="37">
+        <v>1.0178430999999999</v>
+      </c>
+      <c r="T12" s="38">
+        <v>-8.1708750000000006</v>
+      </c>
+      <c r="U12" s="25">
+        <v>345</v>
+      </c>
+      <c r="W12">
+        <v>10</v>
+      </c>
+      <c r="X12" s="25">
+        <v>5</v>
+      </c>
+      <c r="Y12" s="25">
+        <v>6</v>
+      </c>
+      <c r="Z12" s="25">
+        <v>1200</v>
+      </c>
+      <c r="AA12" s="26">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="AB12" s="26">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="AC12" s="26">
+        <v>4.3400000000000001E-2</v>
+      </c>
+      <c r="AD12" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="27"/>
+      <c r="AF12">
+        <f>AB12*zb/wb</f>
+        <v>8.208814077322232E-3</v>
+      </c>
+      <c r="AG12">
+        <f>AC12*sb/wb/kvb/kvb</f>
+        <v>9.672092039751113E-8</v>
+      </c>
+      <c r="AH12">
+        <f t="shared" si="2"/>
+        <v>291.32650544792125</v>
+      </c>
+      <c r="AI12" s="23">
+        <f t="shared" si="3"/>
+        <v>28.177367743113486</v>
+      </c>
+      <c r="AJ12" s="23">
+        <f>0.000001*AI12*mips</f>
+        <v>5.0719261937604276</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36">
+      <c r="B13" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13">
+        <f>SUM(C3:C12)</f>
+        <v>6297.8710000000001</v>
+      </c>
+      <c r="F13">
+        <f>SUM(F3:F12)</f>
+        <v>7367</v>
+      </c>
+      <c r="G13"/>
+      <c r="H13">
+        <f>SUM(H3:H12)</f>
+        <v>6170.326</v>
+      </c>
+      <c r="J13" t="s">
+        <v>94</v>
+      </c>
+      <c r="L13" s="40">
+        <f>SUM(L3:L12)</f>
+        <v>6192.16</v>
+      </c>
+      <c r="P13" s="25">
+        <v>11</v>
+      </c>
+      <c r="Q13" s="27">
+        <v>0</v>
+      </c>
+      <c r="R13" s="27">
+        <v>0</v>
+      </c>
+      <c r="S13" s="37">
+        <v>1.0133858</v>
+      </c>
+      <c r="T13" s="38">
+        <v>-8.9369662999999999</v>
+      </c>
+      <c r="U13" s="25">
+        <v>345</v>
+      </c>
+      <c r="W13">
+        <v>11</v>
+      </c>
+      <c r="X13" s="25">
+        <v>5</v>
+      </c>
+      <c r="Y13" s="25">
+        <v>8</v>
+      </c>
+      <c r="Z13" s="27">
+        <v>900</v>
+      </c>
+      <c r="AA13" s="26">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="AB13" s="26">
+        <v>1.12E-2</v>
+      </c>
+      <c r="AC13" s="26">
+        <v>0.14760000000000001</v>
+      </c>
+      <c r="AD13" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="27"/>
+      <c r="AF13">
+        <f>AB13*zb/wb</f>
+        <v>3.5361045256157311E-2</v>
+      </c>
+      <c r="AG13">
+        <f>AC13*sb/wb/kvb/kvb</f>
+        <v>3.2894027305697341E-7</v>
+      </c>
+      <c r="AH13">
+        <f t="shared" si="2"/>
+        <v>327.87176813727558</v>
+      </c>
+      <c r="AI13" s="23">
+        <f t="shared" si="3"/>
+        <v>107.8502289387481</v>
+      </c>
+      <c r="AJ13" s="23">
+        <f>0.000001*AI13*mips</f>
+        <v>19.413041208974658</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36">
+      <c r="B14" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="5">
+        <f>Q42</f>
+        <v>6254.2300000000005</v>
+      </c>
+      <c r="J14" t="s">
+        <v>93</v>
+      </c>
+      <c r="L14" s="41">
+        <v>6097</v>
+      </c>
+      <c r="P14" s="25">
+        <v>12</v>
+      </c>
+      <c r="Q14" s="27">
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="R14" s="27">
+        <v>88</v>
+      </c>
+      <c r="S14" s="37">
+        <v>1.000815</v>
+      </c>
+      <c r="T14" s="38">
+        <v>-8.9988235999999997</v>
+      </c>
+      <c r="U14" s="25">
+        <v>345</v>
+      </c>
+      <c r="W14">
+        <v>12</v>
+      </c>
+      <c r="X14" s="25">
+        <v>6</v>
+      </c>
+      <c r="Y14" s="25">
+        <v>7</v>
+      </c>
+      <c r="Z14" s="27">
+        <v>900</v>
+      </c>
+      <c r="AA14" s="26">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="AB14" s="26">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="AC14" s="26">
+        <v>0.113</v>
+      </c>
+      <c r="AD14" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="27"/>
+      <c r="AF14">
+        <f>AB14*zb/wb</f>
+        <v>2.9046572888986363E-2</v>
+      </c>
+      <c r="AG14">
+        <f>AC14*sb/wb/kvb/kvb</f>
+        <v>2.5183096785527099E-7</v>
+      </c>
+      <c r="AH14">
+        <f t="shared" si="2"/>
+        <v>339.61970630619243</v>
+      </c>
+      <c r="AI14" s="23">
+        <f t="shared" si="3"/>
+        <v>85.526759341811314</v>
+      </c>
+      <c r="AJ14" s="23">
+        <f>0.000001*AI14*mips</f>
+        <v>15.394816681526034</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36">
+      <c r="B15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="23">
+        <f>C13-C14</f>
+        <v>43.640999999999622</v>
+      </c>
+      <c r="J15" t="s">
+        <v>95</v>
+      </c>
+      <c r="L15" s="41">
+        <f>L13-L14</f>
+        <v>95.159999999999854</v>
+      </c>
+      <c r="P15" s="25">
+        <v>13</v>
+      </c>
+      <c r="Q15" s="27">
+        <v>0</v>
+      </c>
+      <c r="R15" s="27">
+        <v>0</v>
+      </c>
+      <c r="S15" s="37">
+        <v>1.014923</v>
+      </c>
+      <c r="T15" s="38">
+        <v>-8.9299271999999998</v>
+      </c>
+      <c r="U15" s="25">
+        <v>345</v>
+      </c>
+      <c r="W15">
+        <v>13</v>
+      </c>
+      <c r="X15" s="25">
+        <v>6</v>
+      </c>
+      <c r="Y15" s="25">
+        <v>11</v>
+      </c>
+      <c r="Z15" s="27">
+        <v>480</v>
+      </c>
+      <c r="AA15" s="26">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="AB15" s="26">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="AC15" s="26">
+        <v>0.1389</v>
+      </c>
+      <c r="AD15" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="27"/>
+      <c r="AF15">
+        <f>AB15*zb/wb</f>
+        <v>2.5889336705400893E-2</v>
+      </c>
+      <c r="AG15">
+        <f>AC15*sb/wb/kvb/kvb</f>
+        <v>3.0955151712475335E-7</v>
+      </c>
+      <c r="AH15">
+        <f t="shared" si="2"/>
+        <v>289.19713983914977</v>
+      </c>
+      <c r="AI15" s="23">
+        <f t="shared" si="3"/>
+        <v>89.521413385348254</v>
+      </c>
+      <c r="AJ15" s="23">
+        <f>0.000001*AI15*mips</f>
+        <v>16.113854409362684</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36">
+      <c r="P16" s="25">
+        <v>14</v>
+      </c>
+      <c r="Q16" s="27">
+        <v>0</v>
+      </c>
+      <c r="R16" s="27">
+        <v>0</v>
+      </c>
+      <c r="S16" s="37">
+        <v>1.012319</v>
+      </c>
+      <c r="T16" s="38">
+        <v>-10.715294999999999</v>
+      </c>
+      <c r="U16" s="25">
+        <v>345</v>
+      </c>
+      <c r="W16">
+        <v>14</v>
+      </c>
+      <c r="X16" s="25">
+        <v>6</v>
+      </c>
+      <c r="Y16" s="25">
+        <v>31</v>
+      </c>
+      <c r="Z16" s="25">
+        <v>1800</v>
+      </c>
+      <c r="AA16" s="25">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="26">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AC16" s="25">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="27">
+        <v>1.07</v>
+      </c>
+      <c r="AE16" s="27"/>
+      <c r="AF16">
+        <f>AB16*zb/wb</f>
+        <v>7.8930904589636849E-2</v>
+      </c>
+      <c r="AG16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="16:36">
+      <c r="P17" s="25">
+        <v>15</v>
+      </c>
+      <c r="Q17" s="27">
+        <v>320</v>
+      </c>
+      <c r="R17" s="27">
+        <v>153</v>
+      </c>
+      <c r="S17" s="37">
+        <v>1.0161853999999999</v>
+      </c>
+      <c r="T17" s="38">
+        <v>-11.345399</v>
+      </c>
+      <c r="U17" s="25">
+        <v>345</v>
+      </c>
+      <c r="W17">
+        <v>15</v>
+      </c>
+      <c r="X17" s="25">
+        <v>7</v>
+      </c>
+      <c r="Y17" s="25">
+        <v>8</v>
+      </c>
+      <c r="Z17" s="27">
+        <v>900</v>
+      </c>
+      <c r="AA17" s="26">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="AB17" s="26">
+        <v>4.5999999999999999E-3</v>
+      </c>
+      <c r="AC17" s="26">
+        <v>7.8E-2</v>
+      </c>
+      <c r="AD17" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="27"/>
+      <c r="AF17">
+        <f>AB17*zb/wb</f>
+        <v>1.4523286444493182E-2</v>
+      </c>
+      <c r="AG17">
+        <f>AC17*sb/wb/kvb/kvb</f>
+        <v>1.7383022559921359E-7</v>
+      </c>
+      <c r="AH17">
+        <f t="shared" ref="AH17:AH21" si="4">SQRT(AF17/AG17)</f>
+        <v>289.04789079506691</v>
+      </c>
+      <c r="AI17" s="23">
+        <f t="shared" ref="AI17:AI21" si="5">1000000*SQRT(AF17*AG17)</f>
+        <v>50.245260065883329</v>
+      </c>
+      <c r="AJ17" s="23">
+        <f>0.000001*AI17*mips</f>
+        <v>9.0441468118589992</v>
+      </c>
+    </row>
+    <row r="18" spans="16:36">
+      <c r="P18" s="25">
+        <v>16</v>
+      </c>
+      <c r="Q18" s="27">
+        <v>329</v>
+      </c>
+      <c r="R18" s="27">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="S18" s="37">
+        <v>1.0325203000000001</v>
+      </c>
+      <c r="T18" s="38">
+        <v>-10.033348</v>
+      </c>
+      <c r="U18" s="25">
+        <v>345</v>
+      </c>
+      <c r="W18">
+        <v>16</v>
+      </c>
+      <c r="X18" s="25">
+        <v>8</v>
+      </c>
+      <c r="Y18" s="25">
+        <v>9</v>
+      </c>
+      <c r="Z18" s="27">
+        <v>900</v>
+      </c>
+      <c r="AA18" s="26">
+        <v>2.3E-3</v>
+      </c>
+      <c r="AB18" s="26">
+        <v>3.6299999999999999E-2</v>
+      </c>
+      <c r="AC18" s="26">
+        <v>0.38040000000000002</v>
+      </c>
+      <c r="AD18" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="27"/>
+      <c r="AF18">
+        <f>AB18*zb/wb</f>
+        <v>0.11460767346415271</v>
+      </c>
+      <c r="AG18">
+        <f>AC18*sb/wb/kvb/kvb</f>
+        <v>8.4775663869154935E-7</v>
+      </c>
+      <c r="AH18">
+        <f t="shared" si="4"/>
+        <v>367.68105109347408</v>
+      </c>
+      <c r="AI18" s="23">
+        <f t="shared" si="5"/>
+        <v>311.70405198557938</v>
+      </c>
+      <c r="AJ18" s="23">
+        <f>0.000001*AI18*mips</f>
+        <v>56.106729357404284</v>
+      </c>
+    </row>
+    <row r="19" spans="16:36">
+      <c r="P19" s="25">
+        <v>17</v>
+      </c>
+      <c r="Q19" s="27">
+        <v>0</v>
+      </c>
+      <c r="R19" s="27">
+        <v>0</v>
+      </c>
+      <c r="S19" s="37">
+        <v>1.0342365</v>
+      </c>
+      <c r="T19" s="38">
+        <v>-11.116436</v>
+      </c>
+      <c r="U19" s="25">
+        <v>345</v>
+      </c>
+      <c r="W19">
+        <v>17</v>
+      </c>
+      <c r="X19" s="25">
+        <v>9</v>
+      </c>
+      <c r="Y19" s="25">
+        <v>39</v>
+      </c>
+      <c r="Z19" s="27">
+        <v>900</v>
+      </c>
+      <c r="AA19" s="26">
+        <v>1E-3</v>
+      </c>
+      <c r="AB19" s="26">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AC19" s="26">
+        <v>1.2</v>
+      </c>
+      <c r="AD19" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE19" s="27"/>
+      <c r="AF19">
+        <f>AB19*zb/wb</f>
+        <v>7.8930904589636849E-2</v>
+      </c>
+      <c r="AG19">
+        <f>AC19*sb/wb/kvb/kvb</f>
+        <v>2.6743111630648242E-6</v>
+      </c>
+      <c r="AH19">
+        <f t="shared" si="4"/>
+        <v>171.79778947573803</v>
+      </c>
+      <c r="AI19" s="23">
+        <f t="shared" si="5"/>
+        <v>459.44074618482676</v>
+      </c>
+      <c r="AJ19" s="23">
+        <f>0.000001*AI19*mips</f>
+        <v>82.699334313268807</v>
+      </c>
+    </row>
+    <row r="20" spans="16:36">
+      <c r="P20" s="25">
+        <v>18</v>
+      </c>
+      <c r="Q20" s="27">
+        <v>158</v>
+      </c>
+      <c r="R20" s="27">
+        <v>30</v>
+      </c>
+      <c r="S20" s="37">
+        <v>1.0315726000000001</v>
+      </c>
+      <c r="T20" s="38">
+        <v>-11.986167999999999</v>
+      </c>
+      <c r="U20" s="25">
+        <v>345</v>
+      </c>
+      <c r="W20">
+        <v>18</v>
+      </c>
+      <c r="X20" s="25">
+        <v>10</v>
+      </c>
+      <c r="Y20" s="25">
+        <v>11</v>
+      </c>
+      <c r="Z20" s="27">
+        <v>600</v>
+      </c>
+      <c r="AA20" s="26">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="AB20" s="26">
+        <v>4.3E-3</v>
+      </c>
+      <c r="AC20" s="26">
+        <v>7.2900000000000006E-2</v>
+      </c>
+      <c r="AD20" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="27"/>
+      <c r="AF20">
+        <f>AB20*zb/wb</f>
+        <v>1.3576115589417539E-2</v>
+      </c>
+      <c r="AG20">
+        <f>AC20*sb/wb/kvb/kvb</f>
+        <v>1.6246440315618811E-7</v>
+      </c>
+      <c r="AH20">
+        <f t="shared" si="4"/>
+        <v>289.07374827964651</v>
+      </c>
+      <c r="AI20" s="23">
+        <f t="shared" si="5"/>
+        <v>46.96419398237493</v>
+      </c>
+      <c r="AJ20" s="23">
+        <f>0.000001*AI20*mips</f>
+        <v>8.4535549168274873</v>
+      </c>
+    </row>
+    <row r="21" spans="16:36">
+      <c r="P21" s="25">
+        <v>19</v>
+      </c>
+      <c r="Q21" s="27">
+        <v>0</v>
+      </c>
+      <c r="R21" s="27">
+        <v>0</v>
+      </c>
+      <c r="S21" s="37">
+        <v>1.0501068</v>
+      </c>
+      <c r="T21" s="38">
+        <v>-5.4100729000000003</v>
+      </c>
+      <c r="U21" s="25">
+        <v>345</v>
+      </c>
+      <c r="W21">
+        <v>19</v>
+      </c>
+      <c r="X21" s="25">
+        <v>10</v>
+      </c>
+      <c r="Y21" s="25">
+        <v>13</v>
+      </c>
+      <c r="Z21" s="27">
+        <v>600</v>
+      </c>
+      <c r="AA21" s="26">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="AB21" s="26">
+        <v>4.3E-3</v>
+      </c>
+      <c r="AC21" s="26">
+        <v>7.2900000000000006E-2</v>
+      </c>
+      <c r="AD21" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE21" s="27"/>
+      <c r="AF21">
+        <f>AB21*zb/wb</f>
+        <v>1.3576115589417539E-2</v>
+      </c>
+      <c r="AG21">
+        <f>AC21*sb/wb/kvb/kvb</f>
+        <v>1.6246440315618811E-7</v>
+      </c>
+      <c r="AH21">
+        <f t="shared" si="4"/>
+        <v>289.07374827964651</v>
+      </c>
+      <c r="AI21" s="23">
+        <f t="shared" si="5"/>
+        <v>46.96419398237493</v>
+      </c>
+      <c r="AJ21" s="23">
+        <f>0.000001*AI21*mips</f>
+        <v>8.4535549168274873</v>
+      </c>
+    </row>
+    <row r="22" spans="16:36">
+      <c r="P22" s="25">
+        <v>20</v>
+      </c>
+      <c r="Q22" s="27">
+        <v>680</v>
+      </c>
+      <c r="R22" s="27">
+        <v>103</v>
+      </c>
+      <c r="S22" s="37">
+        <v>0.99101054</v>
+      </c>
+      <c r="T22" s="38">
+        <v>-6.8211782999999997</v>
+      </c>
+      <c r="U22" s="25">
+        <v>345</v>
+      </c>
+      <c r="W22">
+        <v>20</v>
+      </c>
+      <c r="X22" s="25">
+        <v>10</v>
+      </c>
+      <c r="Y22" s="25">
+        <v>32</v>
+      </c>
+      <c r="Z22" s="27">
+        <v>900</v>
+      </c>
+      <c r="AA22" s="25">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="26">
+        <v>0.02</v>
+      </c>
+      <c r="AC22" s="25">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="27">
+        <v>1.07</v>
+      </c>
+      <c r="AE22" s="27"/>
+      <c r="AF22">
+        <f>AB22*zb/wb</f>
+        <v>6.314472367170948E-2</v>
+      </c>
+      <c r="AG22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="16:36">
+      <c r="P23" s="25">
+        <v>21</v>
+      </c>
+      <c r="Q23" s="27">
+        <v>274</v>
+      </c>
+      <c r="R23" s="27">
+        <v>115</v>
+      </c>
+      <c r="S23" s="37">
+        <v>1.0323192000000001</v>
+      </c>
+      <c r="T23" s="38">
+        <v>-7.6287460999999999</v>
+      </c>
+      <c r="U23" s="25">
+        <v>345</v>
+      </c>
+      <c r="W23">
+        <v>21</v>
+      </c>
+      <c r="X23" s="25">
+        <v>12</v>
+      </c>
+      <c r="Y23" s="25">
+        <v>11</v>
+      </c>
+      <c r="Z23" s="27">
+        <v>500</v>
+      </c>
+      <c r="AA23" s="26">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="AB23" s="26">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="AC23" s="25">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="26">
+        <v>1.006</v>
+      </c>
+      <c r="AE23" s="26"/>
+      <c r="AF23">
+        <f>AB23*zb/wb</f>
+        <v>0.13733977398596811</v>
+      </c>
+      <c r="AG23" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="16:36">
+      <c r="P24" s="25">
+        <v>22</v>
+      </c>
+      <c r="Q24" s="27">
+        <v>0</v>
+      </c>
+      <c r="R24" s="27">
+        <v>0</v>
+      </c>
+      <c r="S24" s="37">
+        <v>1.0501427000000001</v>
+      </c>
+      <c r="T24" s="38">
+        <v>-3.1831198999999999</v>
+      </c>
+      <c r="U24" s="25">
+        <v>345</v>
+      </c>
+      <c r="W24">
+        <v>22</v>
+      </c>
+      <c r="X24" s="25">
+        <v>12</v>
+      </c>
+      <c r="Y24" s="25">
+        <v>13</v>
+      </c>
+      <c r="Z24" s="27">
+        <v>500</v>
+      </c>
+      <c r="AA24" s="26">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="AB24" s="26">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="AC24" s="25">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="26">
+        <v>1.006</v>
+      </c>
+      <c r="AE24" s="26"/>
+      <c r="AF24">
+        <f>AB24*zb/wb</f>
+        <v>0.13733977398596811</v>
+      </c>
+      <c r="AG24" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="16:36">
+      <c r="P25" s="25">
+        <v>23</v>
+      </c>
+      <c r="Q25" s="26">
+        <v>247.5</v>
+      </c>
+      <c r="R25" s="27">
+        <v>84.6</v>
+      </c>
+      <c r="S25" s="37">
+        <v>1.0451451</v>
+      </c>
+      <c r="T25" s="38">
+        <v>-3.3812763000000001</v>
+      </c>
+      <c r="U25" s="25">
+        <v>345</v>
+      </c>
+      <c r="W25">
+        <v>23</v>
+      </c>
+      <c r="X25" s="25">
+        <v>13</v>
+      </c>
+      <c r="Y25" s="25">
+        <v>14</v>
+      </c>
+      <c r="Z25" s="27">
+        <v>600</v>
+      </c>
+      <c r="AA25" s="26">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="AB25" s="26">
+        <v>1.01E-2</v>
+      </c>
+      <c r="AC25" s="26">
+        <v>0.17230000000000001</v>
+      </c>
+      <c r="AD25" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE25" s="27"/>
+      <c r="AF25">
+        <f>AB25*zb/wb</f>
+        <v>3.1888085454213282E-2</v>
+      </c>
+      <c r="AG25">
+        <f>AC25*sb/wb/kvb/kvb</f>
+        <v>3.83986511163391E-7</v>
+      </c>
+      <c r="AH25">
+        <f t="shared" ref="AH25:AH33" si="6">SQRT(AF25/AG25)</f>
+        <v>288.17495785274275</v>
+      </c>
+      <c r="AI25" s="23">
+        <f t="shared" ref="AI25:AI33" si="7">1000000*SQRT(AF25*AG25)</f>
+        <v>110.65529667053192</v>
+      </c>
+      <c r="AJ25" s="23">
+        <f>0.000001*AI25*mips</f>
+        <v>19.917953400695747</v>
+      </c>
+    </row>
+    <row r="26" spans="16:36">
+      <c r="P26" s="25">
+        <v>24</v>
+      </c>
+      <c r="Q26" s="26">
+        <v>308.60000000000002</v>
+      </c>
+      <c r="R26" s="27">
+        <v>-92.2</v>
+      </c>
+      <c r="S26" s="37">
+        <v>1.038001</v>
+      </c>
+      <c r="T26" s="38">
+        <v>-9.9137585000000001</v>
+      </c>
+      <c r="U26" s="25">
+        <v>345</v>
+      </c>
+      <c r="W26">
+        <v>24</v>
+      </c>
+      <c r="X26" s="25">
+        <v>14</v>
+      </c>
+      <c r="Y26" s="25">
+        <v>15</v>
+      </c>
+      <c r="Z26" s="27">
+        <v>600</v>
+      </c>
+      <c r="AA26" s="26">
+        <v>1.8E-3</v>
+      </c>
+      <c r="AB26" s="26">
+        <v>2.1700000000000001E-2</v>
+      </c>
+      <c r="AC26" s="26">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="AD26" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="27"/>
+      <c r="AF26">
+        <f>AB26*zb/wb</f>
+        <v>6.8512025183804781E-2</v>
+      </c>
+      <c r="AG26">
+        <f>AC26*sb/wb/kvb/kvb</f>
+        <v>8.1566490473477148E-7</v>
+      </c>
+      <c r="AH26">
+        <f t="shared" si="6"/>
+        <v>289.81944094627232</v>
+      </c>
+      <c r="AI26" s="23">
+        <f t="shared" si="7"/>
+        <v>236.39554668972593</v>
+      </c>
+      <c r="AJ26" s="23">
+        <f>0.000001*AI26*mips</f>
+        <v>42.551198404150668</v>
+      </c>
+    </row>
+    <row r="27" spans="16:36">
+      <c r="P27" s="25">
+        <v>25</v>
+      </c>
+      <c r="Q27" s="27">
+        <v>224</v>
+      </c>
+      <c r="R27" s="27">
+        <v>47.2</v>
+      </c>
+      <c r="S27" s="37">
+        <v>1.0576827</v>
+      </c>
+      <c r="T27" s="38">
+        <v>-8.3692354000000009</v>
+      </c>
+      <c r="U27" s="25">
+        <v>345</v>
+      </c>
+      <c r="W27">
+        <v>25</v>
+      </c>
+      <c r="X27" s="25">
+        <v>15</v>
+      </c>
+      <c r="Y27" s="25">
+        <v>16</v>
+      </c>
+      <c r="Z27" s="27">
+        <v>600</v>
+      </c>
+      <c r="AA27" s="26">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="AB27" s="26">
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="AC27" s="26">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="AD27" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="27"/>
+      <c r="AF27">
+        <f>AB27*zb/wb</f>
+        <v>2.9678020125703457E-2</v>
+      </c>
+      <c r="AG27">
+        <f>AC27*sb/wb/kvb/kvb</f>
+        <v>3.8108934073673753E-7</v>
+      </c>
+      <c r="AH27">
+        <f t="shared" si="6"/>
+        <v>279.06415858232879</v>
+      </c>
+      <c r="AI27" s="23">
+        <f t="shared" si="7"/>
+        <v>106.34837621739204</v>
+      </c>
+      <c r="AJ27" s="23">
+        <f>0.000001*AI27*mips</f>
+        <v>19.142707719130566</v>
+      </c>
+    </row>
+    <row r="28" spans="16:36">
+      <c r="P28" s="25">
+        <v>26</v>
+      </c>
+      <c r="Q28" s="27">
+        <v>139</v>
+      </c>
+      <c r="R28" s="27">
+        <v>17</v>
+      </c>
+      <c r="S28" s="37">
+        <v>1.0525613</v>
+      </c>
+      <c r="T28" s="38">
+        <v>-9.4387696000000005</v>
+      </c>
+      <c r="U28" s="25">
+        <v>345</v>
+      </c>
+      <c r="W28">
+        <v>26</v>
+      </c>
+      <c r="X28" s="25">
+        <v>16</v>
+      </c>
+      <c r="Y28" s="25">
+        <v>17</v>
+      </c>
+      <c r="Z28" s="27">
+        <v>600</v>
+      </c>
+      <c r="AA28" s="26">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="AB28" s="26">
+        <v>8.8999999999999999E-3</v>
+      </c>
+      <c r="AC28" s="26">
+        <v>0.13420000000000001</v>
+      </c>
+      <c r="AD28" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="27"/>
+      <c r="AF28">
+        <f>AB28*zb/wb</f>
+        <v>2.809940203391072E-2</v>
+      </c>
+      <c r="AG28">
+        <f>AC28*sb/wb/kvb/kvb</f>
+        <v>2.9907713173608288E-7</v>
+      </c>
+      <c r="AH28">
+        <f t="shared" si="6"/>
+        <v>306.51867218051416</v>
+      </c>
+      <c r="AI28" s="23">
+        <f t="shared" si="7"/>
+        <v>91.672725299300836</v>
+      </c>
+      <c r="AJ28" s="23">
+        <f>0.000001*AI28*mips</f>
+        <v>16.50109055387415</v>
+      </c>
+    </row>
+    <row r="29" spans="16:36">
+      <c r="P29" s="25">
+        <v>27</v>
+      </c>
+      <c r="Q29" s="27">
+        <v>281</v>
+      </c>
+      <c r="R29" s="27">
+        <v>75.5</v>
+      </c>
+      <c r="S29" s="37">
+        <v>1.0383449</v>
+      </c>
+      <c r="T29" s="38">
+        <v>-11.362152</v>
+      </c>
+      <c r="U29" s="25">
+        <v>345</v>
+      </c>
+      <c r="W29">
+        <v>27</v>
+      </c>
+      <c r="X29" s="25">
+        <v>16</v>
+      </c>
+      <c r="Y29" s="25">
+        <v>19</v>
+      </c>
+      <c r="Z29" s="27">
+        <v>600</v>
+      </c>
+      <c r="AA29" s="26">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="AB29" s="26">
+        <v>1.95E-2</v>
+      </c>
+      <c r="AC29" s="26">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="AD29" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE29" s="27"/>
+      <c r="AF29">
+        <f>AB29*zb/wb</f>
+        <v>6.1566105579916743E-2</v>
+      </c>
+      <c r="AG29">
+        <f>AC29*sb/wb/kvb/kvb</f>
+        <v>6.7749216130975552E-7</v>
+      </c>
+      <c r="AH29">
+        <f t="shared" si="6"/>
+        <v>301.45237098018049</v>
+      </c>
+      <c r="AI29" s="23">
+        <f t="shared" si="7"/>
+        <v>204.23161834731269</v>
+      </c>
+      <c r="AJ29" s="23">
+        <f>0.000001*AI29*mips</f>
+        <v>36.761691302516283</v>
+      </c>
+    </row>
+    <row r="30" spans="16:36">
+      <c r="P30" s="25">
+        <v>28</v>
+      </c>
+      <c r="Q30" s="27">
+        <v>206</v>
+      </c>
+      <c r="R30" s="27">
+        <v>27.6</v>
+      </c>
+      <c r="S30" s="37">
+        <v>1.0503737</v>
+      </c>
+      <c r="T30" s="38">
+        <v>-5.9283592000000001</v>
+      </c>
+      <c r="U30" s="25">
+        <v>345</v>
+      </c>
+      <c r="W30">
+        <v>28</v>
+      </c>
+      <c r="X30" s="25">
+        <v>16</v>
+      </c>
+      <c r="Y30" s="25">
+        <v>21</v>
+      </c>
+      <c r="Z30" s="27">
+        <v>600</v>
+      </c>
+      <c r="AA30" s="26">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="AB30" s="26">
+        <v>1.35E-2</v>
+      </c>
+      <c r="AC30" s="26">
+        <v>0.25480000000000003</v>
+      </c>
+      <c r="AD30" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE30" s="27"/>
+      <c r="AF30">
+        <f>AB30*zb/wb</f>
+        <v>4.2622688478403899E-2</v>
+      </c>
+      <c r="AG30">
+        <f>AC30*sb/wb/kvb/kvb</f>
+        <v>5.6784540362409773E-7</v>
+      </c>
+      <c r="AH30">
+        <f t="shared" si="6"/>
+        <v>273.9714842653184</v>
+      </c>
+      <c r="AI30" s="23">
+        <f t="shared" si="7"/>
+        <v>155.57344806413286</v>
+      </c>
+      <c r="AJ30" s="23">
+        <f>0.000001*AI30*mips</f>
+        <v>28.003220651543913</v>
+      </c>
+    </row>
+    <row r="31" spans="16:36">
+      <c r="P31" s="25">
+        <v>29</v>
+      </c>
+      <c r="Q31" s="26">
+        <v>283.5</v>
+      </c>
+      <c r="R31" s="27">
+        <v>26.9</v>
+      </c>
+      <c r="S31" s="37">
+        <v>1.0501149000000001</v>
+      </c>
+      <c r="T31" s="38">
+        <v>-3.1698740999999999</v>
+      </c>
+      <c r="U31" s="25">
+        <v>345</v>
+      </c>
+      <c r="W31">
+        <v>29</v>
+      </c>
+      <c r="X31" s="25">
+        <v>16</v>
+      </c>
+      <c r="Y31" s="25">
+        <v>24</v>
+      </c>
+      <c r="Z31" s="27">
+        <v>600</v>
+      </c>
+      <c r="AA31" s="26">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AB31" s="26">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="AC31" s="26">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="AD31" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE31" s="27"/>
+      <c r="AF31">
+        <f>AB31*zb/wb</f>
+        <v>1.8627693483154299E-2</v>
+      </c>
+      <c r="AG31">
+        <f>AC31*sb/wb/kvb/kvb</f>
+        <v>1.5154429924034006E-7</v>
+      </c>
+      <c r="AH31">
+        <f t="shared" si="6"/>
+        <v>350.59824646280549</v>
+      </c>
+      <c r="AI31" s="23">
+        <f t="shared" si="7"/>
+        <v>53.131165575097896</v>
+      </c>
+      <c r="AJ31" s="23">
+        <f>0.000001*AI31*mips</f>
+        <v>9.56360980351762</v>
+      </c>
+    </row>
+    <row r="32" spans="16:36">
+      <c r="P32" s="25">
+        <v>30</v>
+      </c>
+      <c r="Q32" s="27">
+        <v>0</v>
+      </c>
+      <c r="R32" s="27">
+        <v>0</v>
+      </c>
+      <c r="S32" s="37">
+        <v>1.0499000000000001</v>
+      </c>
+      <c r="T32" s="38">
+        <v>-7.3704745999999997</v>
+      </c>
+      <c r="U32" s="27">
+        <v>20</v>
+      </c>
+      <c r="W32">
+        <v>30</v>
+      </c>
+      <c r="X32" s="25">
+        <v>17</v>
+      </c>
+      <c r="Y32" s="25">
+        <v>18</v>
+      </c>
+      <c r="Z32" s="27">
+        <v>600</v>
+      </c>
+      <c r="AA32" s="26">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="AB32" s="26">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="AC32" s="26">
+        <v>0.13189999999999999</v>
+      </c>
+      <c r="AD32" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE32" s="27"/>
+      <c r="AF32">
+        <f>AB32*zb/wb</f>
+        <v>2.5889336705400893E-2</v>
+      </c>
+      <c r="AG32">
+        <f>AC32*sb/wb/kvb/kvb</f>
+        <v>2.9395136867354191E-7</v>
+      </c>
+      <c r="AH32">
+        <f t="shared" si="6"/>
+        <v>296.77185996156931</v>
+      </c>
+      <c r="AI32" s="23">
+        <f t="shared" si="7"/>
+        <v>87.236494419495997</v>
+      </c>
+      <c r="AJ32" s="23">
+        <f>0.000001*AI32*mips</f>
+        <v>15.702568995509278</v>
+      </c>
+    </row>
+    <row r="33" spans="16:36">
+      <c r="P33" s="25">
+        <v>31</v>
+      </c>
+      <c r="Q33" s="27">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="R33" s="27">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="S33" s="37">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="T33" s="38">
+        <v>0</v>
+      </c>
+      <c r="U33" s="27">
+        <v>20</v>
+      </c>
+      <c r="W33">
+        <v>31</v>
+      </c>
+      <c r="X33" s="25">
+        <v>17</v>
+      </c>
+      <c r="Y33" s="25">
+        <v>27</v>
+      </c>
+      <c r="Z33" s="27">
+        <v>600</v>
+      </c>
+      <c r="AA33" s="26">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="AB33" s="26">
+        <v>1.7299999999999999E-2</v>
+      </c>
+      <c r="AC33" s="26">
+        <v>0.3216</v>
+      </c>
+      <c r="AD33" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE33" s="27"/>
+      <c r="AF33">
+        <f>AB33*zb/wb</f>
+        <v>5.4620185976028697E-2</v>
+      </c>
+      <c r="AG33">
+        <f>AC33*sb/wb/kvb/kvb</f>
+        <v>7.1671539170137281E-7</v>
+      </c>
+      <c r="AH33">
+        <f t="shared" si="6"/>
+        <v>276.05983347476626</v>
+      </c>
+      <c r="AI33" s="23">
+        <f t="shared" si="7"/>
+        <v>197.85633168188284</v>
+      </c>
+      <c r="AJ33" s="23">
+        <f>0.000001*AI33*mips</f>
+        <v>35.61413970273891</v>
+      </c>
+    </row>
+    <row r="34" spans="16:36">
+      <c r="P34" s="25">
+        <v>32</v>
+      </c>
+      <c r="Q34" s="27">
+        <v>0</v>
+      </c>
+      <c r="R34" s="27">
+        <v>0</v>
+      </c>
+      <c r="S34" s="37">
+        <v>0.98409999999999997</v>
+      </c>
+      <c r="T34" s="38">
+        <v>-0.1884374</v>
+      </c>
+      <c r="U34" s="27">
+        <v>20</v>
+      </c>
+      <c r="W34">
+        <v>32</v>
+      </c>
+      <c r="X34" s="25">
+        <v>19</v>
+      </c>
+      <c r="Y34" s="25">
+        <v>20</v>
+      </c>
+      <c r="Z34" s="27">
+        <v>900</v>
+      </c>
+      <c r="AA34" s="26">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="AB34" s="26">
+        <v>1.38E-2</v>
+      </c>
+      <c r="AC34" s="25">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="27">
+        <v>1.06</v>
+      </c>
+      <c r="AE34" s="27"/>
+      <c r="AF34">
+        <f>AB34*zb/wb</f>
+        <v>4.3569859333479545E-2</v>
+      </c>
+      <c r="AG34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="16:36">
+      <c r="P35" s="25">
+        <v>33</v>
+      </c>
+      <c r="Q35" s="27">
+        <v>0</v>
+      </c>
+      <c r="R35" s="27">
+        <v>0</v>
+      </c>
+      <c r="S35" s="37">
+        <v>0.99719999999999998</v>
+      </c>
+      <c r="T35" s="38">
+        <v>-0.19317445</v>
+      </c>
+      <c r="U35" s="27">
+        <v>20</v>
+      </c>
+      <c r="W35">
+        <v>33</v>
+      </c>
+      <c r="X35" s="25">
+        <v>19</v>
+      </c>
+      <c r="Y35" s="25">
+        <v>33</v>
+      </c>
+      <c r="Z35" s="27">
+        <v>900</v>
+      </c>
+      <c r="AA35" s="26">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="AB35" s="26">
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="AC35" s="25">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="27">
+        <v>1.07</v>
+      </c>
+      <c r="AE35" s="27"/>
+      <c r="AF35">
+        <f>AB35*zb/wb</f>
+        <v>4.4832753806913733E-2</v>
+      </c>
+      <c r="AG35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="16:36">
+      <c r="P36" s="25">
+        <v>34</v>
+      </c>
+      <c r="Q36" s="27">
+        <v>0</v>
+      </c>
+      <c r="R36" s="27">
+        <v>0</v>
+      </c>
+      <c r="S36" s="37">
+        <v>1.0123</v>
+      </c>
+      <c r="T36" s="38">
+        <v>-1.631119</v>
+      </c>
+      <c r="U36" s="27">
+        <v>20</v>
+      </c>
+      <c r="W36">
+        <v>34</v>
+      </c>
+      <c r="X36" s="25">
+        <v>20</v>
+      </c>
+      <c r="Y36" s="25">
+        <v>34</v>
+      </c>
+      <c r="Z36" s="27">
+        <v>900</v>
+      </c>
+      <c r="AA36" s="26">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="AB36" s="26">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="AC36" s="25">
+        <v>0</v>
+      </c>
+      <c r="AD36" s="26">
+        <v>1.0089999999999999</v>
+      </c>
+      <c r="AE36" s="26"/>
+      <c r="AF36">
+        <f>AB36*zb/wb</f>
+        <v>5.6830251304538532E-2</v>
+      </c>
+      <c r="AG36" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="16:36">
+      <c r="P37" s="25">
+        <v>35</v>
+      </c>
+      <c r="Q37" s="27">
+        <v>0</v>
+      </c>
+      <c r="R37" s="27">
+        <v>0</v>
+      </c>
+      <c r="S37" s="37">
+        <v>1.0494000000000001</v>
+      </c>
+      <c r="T37" s="38">
+        <v>1.7765069</v>
+      </c>
+      <c r="U37" s="27">
+        <v>20</v>
+      </c>
+      <c r="W37">
+        <v>35</v>
+      </c>
+      <c r="X37" s="25">
+        <v>21</v>
+      </c>
+      <c r="Y37" s="25">
+        <v>22</v>
+      </c>
+      <c r="Z37" s="27">
+        <v>900</v>
+      </c>
+      <c r="AA37" s="26">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="AB37" s="26">
+        <v>1.4E-2</v>
+      </c>
+      <c r="AC37" s="26">
+        <v>0.25650000000000001</v>
+      </c>
+      <c r="AD37" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE37" s="27"/>
+      <c r="AF37">
+        <f>AB37*zb/wb</f>
+        <v>4.4201306570196636E-2</v>
+      </c>
+      <c r="AG37">
+        <f>AC37*sb/wb/kvb/kvb</f>
+        <v>5.7163401110510618E-7</v>
+      </c>
+      <c r="AH37">
+        <f t="shared" ref="AH37:AH38" si="8">SQRT(AF37/AG37)</f>
+        <v>278.07280852702098</v>
+      </c>
+      <c r="AI37" s="23">
+        <f t="shared" ref="AI37:AI38" si="9">1000000*SQRT(AF37*AG37)</f>
+        <v>158.95587491756316</v>
+      </c>
+      <c r="AJ37" s="23">
+        <f>0.000001*AI37*mips</f>
+        <v>28.612057485161369</v>
+      </c>
+    </row>
+    <row r="38" spans="16:36">
+      <c r="P38" s="25">
+        <v>36</v>
+      </c>
+      <c r="Q38" s="27">
+        <v>0</v>
+      </c>
+      <c r="R38" s="27">
+        <v>0</v>
+      </c>
+      <c r="S38" s="37">
+        <v>1.0636000000000001</v>
+      </c>
+      <c r="T38" s="38">
+        <v>4.4684374</v>
+      </c>
+      <c r="U38" s="27">
+        <v>20</v>
+      </c>
+      <c r="W38">
+        <v>36</v>
+      </c>
+      <c r="X38" s="25">
+        <v>22</v>
+      </c>
+      <c r="Y38" s="25">
+        <v>23</v>
+      </c>
+      <c r="Z38" s="27">
+        <v>600</v>
+      </c>
+      <c r="AA38" s="26">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="AB38" s="26">
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="AC38" s="26">
+        <v>0.18459999999999999</v>
+      </c>
+      <c r="AD38" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE38" s="27"/>
+      <c r="AF38">
+        <f>AB38*zb/wb</f>
+        <v>3.0309467362420548E-2</v>
+      </c>
+      <c r="AG38">
+        <f>AC38*sb/wb/kvb/kvb</f>
+        <v>4.1139820058480539E-7</v>
+      </c>
+      <c r="AH38">
+        <f t="shared" si="8"/>
+        <v>271.43006976671626</v>
+      </c>
+      <c r="AI38" s="23">
+        <f t="shared" si="9"/>
+        <v>111.66584228663527</v>
+      </c>
+      <c r="AJ38" s="23">
+        <f>0.000001*AI38*mips</f>
+        <v>20.099851611594346</v>
+      </c>
+    </row>
+    <row r="39" spans="16:36">
+      <c r="P39" s="25">
+        <v>37</v>
+      </c>
+      <c r="Q39" s="27">
+        <v>0</v>
+      </c>
+      <c r="R39" s="27">
+        <v>0</v>
+      </c>
+      <c r="S39" s="37">
+        <v>1.0275000000000001</v>
+      </c>
+      <c r="T39" s="38">
+        <v>-1.5828987999999999</v>
+      </c>
+      <c r="U39" s="27">
+        <v>20</v>
+      </c>
+      <c r="W39">
+        <v>37</v>
+      </c>
+      <c r="X39" s="25">
+        <v>22</v>
+      </c>
+      <c r="Y39" s="25">
+        <v>35</v>
+      </c>
+      <c r="Z39" s="27">
+        <v>900</v>
+      </c>
+      <c r="AA39" s="25">
+        <v>0</v>
+      </c>
+      <c r="AB39" s="26">
+        <v>1.43E-2</v>
+      </c>
+      <c r="AC39" s="25">
+        <v>0</v>
+      </c>
+      <c r="AD39" s="26">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="AE39" s="26"/>
+      <c r="AF39">
+        <f>AB39*zb/wb</f>
+        <v>4.5148477425272282E-2</v>
+      </c>
+      <c r="AG39" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="16:36">
+      <c r="P40" s="25">
+        <v>38</v>
+      </c>
+      <c r="Q40" s="27">
+        <v>0</v>
+      </c>
+      <c r="R40" s="27">
+        <v>0</v>
+      </c>
+      <c r="S40" s="37">
+        <v>1.0265</v>
+      </c>
+      <c r="T40" s="38">
+        <v>3.8928177000000002</v>
+      </c>
+      <c r="U40" s="27">
+        <v>20</v>
+      </c>
+      <c r="W40">
+        <v>38</v>
+      </c>
+      <c r="X40" s="25">
+        <v>23</v>
+      </c>
+      <c r="Y40" s="25">
+        <v>24</v>
+      </c>
+      <c r="Z40" s="27">
+        <v>600</v>
+      </c>
+      <c r="AA40" s="26">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="AB40" s="26">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="AC40" s="26">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="AD40" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE40" s="27"/>
+      <c r="AF40">
+        <f>AB40*zb/wb</f>
+        <v>0.1105032664254916</v>
+      </c>
+      <c r="AG40">
+        <f>AC40*sb/wb/kvb/kvb</f>
+        <v>8.0452194155533466E-7</v>
+      </c>
+      <c r="AH40">
+        <f t="shared" ref="AH40:AH42" si="10">SQRT(AF40/AG40)</f>
+        <v>370.61126114917465</v>
+      </c>
+      <c r="AI40" s="23">
+        <f>1000000*SQRT(AF40*AG40)</f>
+        <v>298.16489138200518</v>
+      </c>
+      <c r="AJ40" s="23">
+        <f>0.000001*AI40*mips</f>
+        <v>53.669680448760928</v>
+      </c>
+    </row>
+    <row r="41" spans="16:36">
+      <c r="P41" s="25">
+        <v>39</v>
+      </c>
+      <c r="Q41" s="27">
+        <v>1104</v>
+      </c>
+      <c r="R41" s="27">
+        <v>250</v>
+      </c>
+      <c r="S41" s="37">
+        <v>1.03</v>
+      </c>
+      <c r="T41" s="38">
+        <v>-14.535256</v>
+      </c>
+      <c r="U41" s="25">
+        <v>345</v>
+      </c>
+      <c r="W41">
+        <v>39</v>
+      </c>
+      <c r="X41" s="25">
+        <v>23</v>
+      </c>
+      <c r="Y41" s="25">
+        <v>36</v>
+      </c>
+      <c r="Z41" s="27">
+        <v>900</v>
+      </c>
+      <c r="AA41" s="26">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="AB41" s="26">
+        <v>2.7199999999999998E-2</v>
+      </c>
+      <c r="AC41" s="25">
+        <v>0</v>
+      </c>
+      <c r="AD41" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE41" s="27"/>
+      <c r="AF41">
+        <f>AB41*zb/wb</f>
+        <v>8.5876824193524895E-2</v>
+      </c>
+      <c r="AG41">
+        <f>AC41*sb/wb/kvb/kvb</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="16:36">
+      <c r="P42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q42">
+        <f>SUM(Q3:Q41)</f>
+        <v>6254.2300000000005</v>
+      </c>
+      <c r="R42">
+        <f>SUM(R3:R41)</f>
+        <v>1387.1</v>
+      </c>
+      <c r="W42">
+        <v>40</v>
+      </c>
+      <c r="X42" s="25">
+        <v>25</v>
+      </c>
+      <c r="Y42" s="25">
+        <v>26</v>
+      </c>
+      <c r="Z42" s="27">
+        <v>600</v>
+      </c>
+      <c r="AA42" s="26">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="AB42" s="26">
+        <v>3.2300000000000002E-2</v>
+      </c>
+      <c r="AC42" s="26">
+        <v>0.53100000000000003</v>
+      </c>
+      <c r="AD42" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE42" s="27"/>
+      <c r="AF42">
+        <f>AB42*zb/wb</f>
+        <v>0.10197872872981081</v>
+      </c>
+      <c r="AG42">
+        <f>AC42*sb/wb/kvb/kvb</f>
+        <v>1.1833826896561849E-6</v>
+      </c>
+      <c r="AH42">
+        <f t="shared" si="10"/>
+        <v>293.55683100493678</v>
+      </c>
+      <c r="AI42" s="23">
+        <f>1000000*SQRT(AF42*AG42)</f>
+        <v>347.39007224156819</v>
+      </c>
+      <c r="AJ42" s="23">
+        <f>0.000001*AI42*mips</f>
+        <v>62.530213003482274</v>
+      </c>
+    </row>
+    <row r="43" spans="16:36">
+      <c r="W43">
+        <v>41</v>
+      </c>
+      <c r="X43" s="25">
+        <v>25</v>
+      </c>
+      <c r="Y43" s="25">
+        <v>37</v>
+      </c>
+      <c r="Z43" s="27">
+        <v>900</v>
+      </c>
+      <c r="AA43" s="26">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="AB43" s="26">
+        <v>2.3199999999999998E-2</v>
+      </c>
+      <c r="AC43" s="25">
+        <v>0</v>
+      </c>
+      <c r="AD43" s="26">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="AE43" s="26"/>
+      <c r="AF43">
+        <f>AB43*zb/wb</f>
+        <v>7.3247879459182999E-2</v>
+      </c>
+      <c r="AG43" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="16:36">
+      <c r="W44">
+        <v>42</v>
+      </c>
+      <c r="X44" s="25">
+        <v>26</v>
+      </c>
+      <c r="Y44" s="25">
+        <v>27</v>
+      </c>
+      <c r="Z44" s="27">
+        <v>600</v>
+      </c>
+      <c r="AA44" s="26">
+        <v>1.4E-3</v>
+      </c>
+      <c r="AB44" s="26">
+        <v>1.47E-2</v>
+      </c>
+      <c r="AC44" s="26">
+        <v>0.23960000000000001</v>
+      </c>
+      <c r="AD44" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE44" s="27"/>
+      <c r="AF44">
+        <f>AB44*zb/wb</f>
+        <v>4.641137189870647E-2</v>
+      </c>
+      <c r="AG44">
+        <f>AC44*sb/wb/kvb/kvb</f>
+        <v>5.339707955586099E-7</v>
+      </c>
+      <c r="AH44">
+        <f t="shared" ref="AH44:AH47" si="11">SQRT(AF44/AG44)</f>
+        <v>294.81763001852727</v>
+      </c>
+      <c r="AI44" s="23">
+        <f t="shared" ref="AI44:AI47" si="12">1000000*SQRT(AF44*AG44)</f>
+        <v>157.42400444569694</v>
+      </c>
+      <c r="AJ44" s="23">
+        <f>0.000001*AI44*mips</f>
+        <v>28.336320800225447</v>
+      </c>
+    </row>
+    <row r="45" spans="16:36">
+      <c r="W45">
+        <v>43</v>
+      </c>
+      <c r="X45" s="25">
+        <v>26</v>
+      </c>
+      <c r="Y45" s="25">
+        <v>28</v>
+      </c>
+      <c r="Z45" s="27">
+        <v>600</v>
+      </c>
+      <c r="AA45" s="26">
+        <v>4.3E-3</v>
+      </c>
+      <c r="AB45" s="26">
+        <v>4.7399999999999998E-2</v>
+      </c>
+      <c r="AC45" s="26">
+        <v>0.7802</v>
+      </c>
+      <c r="AD45" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE45" s="27"/>
+      <c r="AF45">
+        <f>AB45*zb/wb</f>
+        <v>0.14965299510195146</v>
+      </c>
+      <c r="AG45">
+        <f>AC45*sb/wb/kvb/kvb</f>
+        <v>1.7387479745193131E-6</v>
+      </c>
+      <c r="AH45">
+        <f t="shared" si="11"/>
+        <v>293.37586830845873</v>
+      </c>
+      <c r="AI45" s="23">
+        <f t="shared" si="12"/>
+        <v>510.10669679417737</v>
+      </c>
+      <c r="AJ45" s="23">
+        <f>0.000001*AI45*mips</f>
+        <v>91.819205422951924</v>
+      </c>
+    </row>
+    <row r="46" spans="16:36">
+      <c r="W46">
+        <v>44</v>
+      </c>
+      <c r="X46" s="25">
+        <v>26</v>
+      </c>
+      <c r="Y46" s="25">
+        <v>29</v>
+      </c>
+      <c r="Z46" s="27">
+        <v>600</v>
+      </c>
+      <c r="AA46" s="26">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="AB46" s="26">
+        <v>6.25E-2</v>
+      </c>
+      <c r="AC46" s="26">
+        <v>1.0289999999999999</v>
+      </c>
+      <c r="AD46" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE46" s="27"/>
+      <c r="AF46">
+        <f>AB46*zb/wb</f>
+        <v>0.19732726147409213</v>
+      </c>
+      <c r="AG46">
+        <f>AC46*sb/wb/kvb/kvb</f>
+        <v>2.2932218223280869E-6</v>
+      </c>
+      <c r="AH46">
+        <f t="shared" si="11"/>
+        <v>293.33947571687042</v>
+      </c>
+      <c r="AI46" s="23">
+        <f t="shared" si="12"/>
+        <v>672.69248706420717</v>
+      </c>
+      <c r="AJ46" s="23">
+        <f>0.000001*AI46*mips</f>
+        <v>121.08464767155728</v>
+      </c>
+    </row>
+    <row r="47" spans="16:36">
+      <c r="W47">
+        <v>45</v>
+      </c>
+      <c r="X47" s="25">
+        <v>28</v>
+      </c>
+      <c r="Y47" s="25">
+        <v>29</v>
+      </c>
+      <c r="Z47" s="27">
+        <v>600</v>
+      </c>
+      <c r="AA47" s="26">
+        <v>1.4E-3</v>
+      </c>
+      <c r="AB47" s="26">
+        <v>1.5100000000000001E-2</v>
+      </c>
+      <c r="AC47" s="26">
+        <v>0.249</v>
+      </c>
+      <c r="AD47" s="27">
+        <v>0</v>
+      </c>
+      <c r="AE47" s="27"/>
+      <c r="AF47">
+        <f>AB47*zb/wb</f>
+        <v>4.7674266372140665E-2</v>
+      </c>
+      <c r="AG47">
+        <f>AC47*sb/wb/kvb/kvb</f>
+        <v>5.5491956633595096E-7</v>
+      </c>
+      <c r="AH47">
+        <f t="shared" si="11"/>
+        <v>293.10753981188941</v>
+      </c>
+      <c r="AI47" s="23">
+        <f t="shared" si="12"/>
+        <v>162.65110888221116</v>
+      </c>
+      <c r="AJ47" s="23">
+        <f>0.000001*AI47*mips</f>
+        <v>29.277199598798006</v>
+      </c>
+    </row>
+    <row r="48" spans="16:36">
+      <c r="W48">
+        <v>46</v>
+      </c>
+      <c r="X48" s="25">
+        <v>29</v>
+      </c>
+      <c r="Y48" s="25">
+        <v>38</v>
+      </c>
+      <c r="Z48" s="25">
+        <v>1200</v>
+      </c>
+      <c r="AA48" s="26">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="AB48" s="26">
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="AC48" s="25">
+        <v>0</v>
+      </c>
+      <c r="AD48" s="26">
+        <v>1.0249999999999999</v>
+      </c>
+      <c r="AE48" s="26"/>
+      <c r="AF48">
+        <f>AB48*zb/wb</f>
+        <v>4.9252884463933388E-2</v>
+      </c>
+      <c r="AG48" s="26">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="W1:AD1"/>
+    <mergeCell ref="H1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updating EMTP models to account for plant reactance
</commit_message>
<xml_diff>
--- a/emt-bootcamp/Support/EMTBootCamp.xlsx
+++ b/emt-bootcamp/Support/EMTBootCamp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\i2x\emt-bootcamp\Support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9B5C34-E604-46E6-AA16-D3922A7E10BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780D16BA-B075-4B4B-8308-0579915B75EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="5060" windowWidth="30940" windowHeight="13810" activeTab="6" xr2:uid="{A8C2E3F1-142E-440E-A762-DE7B4CF8E5D3}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="11232" activeTab="3" xr2:uid="{A8C2E3F1-142E-440E-A762-DE7B4CF8E5D3}"/>
   </bookViews>
   <sheets>
     <sheet name="COMTRADE" sheetId="1" r:id="rId1"/>
@@ -37,12 +37,13 @@
     <definedName name="VpuMax">COMTRADE!$N$9</definedName>
     <definedName name="Vscale">COMTRADE!$N$6</definedName>
     <definedName name="wb">IEEE39m!$AH$1</definedName>
-    <definedName name="XS" localSheetId="3">StepSCR!$J$6</definedName>
+    <definedName name="XS" localSheetId="3">StepSCR!$K$6</definedName>
     <definedName name="XS" localSheetId="2">Weak!$F$5</definedName>
     <definedName name="XS">Source!$F$5</definedName>
     <definedName name="zb">IEEE39m!$AI$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="180">
   <si>
     <t>Name</t>
   </si>
@@ -681,6 +682,33 @@
   </si>
   <si>
     <t>dl</t>
+  </si>
+  <si>
+    <r>
+      <t>Rs [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+        <family val="1"/>
+        <charset val="2"/>
+      </rPr>
+      <t>W</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>]</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -884,10 +912,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1208,19 +1236,19 @@
       <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="8.7265625" customWidth="1"/>
-    <col min="5" max="5" width="7.6328125" customWidth="1"/>
-    <col min="6" max="6" width="8.54296875" customWidth="1"/>
-    <col min="7" max="7" width="8.6328125" customWidth="1"/>
+    <col min="4" max="4" width="8.77734375" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="11" max="11" width="10.453125" customWidth="1"/>
-    <col min="12" max="12" width="5.81640625" customWidth="1"/>
-    <col min="13" max="13" width="9.6328125" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" customWidth="1"/>
+    <col min="12" max="12" width="5.77734375" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="29">
+    <row r="1" spans="1:14" ht="28.8">
       <c r="A1" s="14" t="s">
         <v>43</v>
       </c>
@@ -1723,10 +1751,10 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.6328125" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1873,10 +1901,10 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.6328125" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2017,28 +2045,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70A51ED4-A577-4B06-8042-A04C86E2D43B}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.36328125" customWidth="1"/>
-    <col min="5" max="8" width="9.54296875" customWidth="1"/>
+    <col min="2" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="8" width="9.5546875" customWidth="1"/>
+    <col min="9" max="9" width="4.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="D1" s="1" t="s">
+    <row r="1" spans="1:11">
+      <c r="D1" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E1" s="44"/>
+      <c r="F1" s="44" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="G1" s="44"/>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="4" t="s">
         <v>53</v>
       </c>
@@ -2060,24 +2091,27 @@
       <c r="G2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="1" t="s">
+      <c r="H2" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>230</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" s="6">
         <v>20</v>
       </c>
       <c r="B3" s="21">
-        <f t="shared" ref="B3:B11" si="0">A3*J$3</f>
+        <f t="shared" ref="B3:B11" si="0">A3*K$3</f>
         <v>2000</v>
       </c>
       <c r="C3" s="20">
-        <f t="shared" ref="C3:C11" si="1">J$2*J$2/B3</f>
+        <f t="shared" ref="C3:C11" si="1">K$2*K$2/B3</f>
         <v>26.45</v>
       </c>
       <c r="D3" s="24">
@@ -2095,14 +2129,15 @@
         <v>-73.679999999999993</v>
       </c>
       <c r="H3" s="22"/>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="22"/>
+      <c r="J3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4" s="6">
         <v>10</v>
       </c>
@@ -2131,9 +2166,10 @@
         <v>-47.23</v>
       </c>
       <c r="H4" s="22"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="I4" s="22"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="6">
         <v>5</v>
       </c>
@@ -2161,10 +2197,14 @@
         <f t="shared" si="3"/>
         <v>5.6700000000000017</v>
       </c>
-      <c r="H5" s="22"/>
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="H5" s="22">
+        <f>G5/11.433</f>
+        <v>0.49593282602991356</v>
+      </c>
+      <c r="I5" s="22"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -2192,11 +2232,15 @@
         <f t="shared" si="3"/>
         <v>32.120000000000005</v>
       </c>
-      <c r="H6" s="22"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="23"/>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="H6" s="22">
+        <f t="shared" ref="H6:H11" si="5">G6/11.433</f>
+        <v>2.8094113531006739</v>
+      </c>
+      <c r="I6" s="22"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="23"/>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="6">
         <v>3</v>
       </c>
@@ -2224,10 +2268,14 @@
         <f t="shared" si="3"/>
         <v>76.203333333333347</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="H7" s="22">
+        <f t="shared" si="5"/>
+        <v>6.6652088982186086</v>
+      </c>
+      <c r="I7" s="22"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="6">
         <v>2.5</v>
       </c>
@@ -2255,10 +2303,14 @@
         <f t="shared" si="3"/>
         <v>111.47</v>
       </c>
-      <c r="H8" s="22"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="H8" s="22">
+        <f t="shared" si="5"/>
+        <v>9.7498469343129539</v>
+      </c>
+      <c r="I8" s="22"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="6">
         <v>2</v>
       </c>
@@ -2286,10 +2338,14 @@
         <f t="shared" si="3"/>
         <v>164.37</v>
       </c>
-      <c r="H9" s="22"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="H9" s="22">
+        <f t="shared" si="5"/>
+        <v>14.376803988454474</v>
+      </c>
+      <c r="I9" s="22"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="6">
         <v>1.5</v>
       </c>
@@ -2306,7 +2362,7 @@
         <v>74.06</v>
       </c>
       <c r="E10" s="22">
-        <f t="shared" ref="E10" si="5">C10-D10</f>
+        <f t="shared" ref="E10" si="6">C10-D10</f>
         <v>278.60666666666668</v>
       </c>
       <c r="F10" s="20">
@@ -2314,13 +2370,17 @@
         <v>100.13</v>
       </c>
       <c r="G10" s="22">
-        <f t="shared" ref="G10" si="6">C10-F10</f>
+        <f t="shared" ref="G10" si="7">C10-F10</f>
         <v>252.53666666666669</v>
       </c>
-      <c r="H10" s="22"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="H10" s="22">
+        <f t="shared" si="5"/>
+        <v>22.088399078690344</v>
+      </c>
+      <c r="I10" s="22"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="6">
         <v>1</v>
       </c>
@@ -2348,27 +2408,36 @@
         <f t="shared" si="3"/>
         <v>428.87</v>
       </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="H11" s="22">
+        <f t="shared" si="5"/>
+        <v>37.511589259162079</v>
+      </c>
+      <c r="I11" s="22"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:11">
       <c r="D12" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E12" s="22">
-        <f>$J$2*$J$2/$D$3/100</f>
+        <f>$K$2*$K$2/$D$3/100</f>
         <v>7.1428571428571423</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G12" s="22">
-        <f>$J$2*$J$2/$F$3/100</f>
+        <f>$K$2*$K$2/$F$3/100</f>
         <v>5.283131928492959</v>
       </c>
       <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -2383,62 +2452,62 @@
       <selection pane="bottomLeft" activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="6" width="8.7265625" style="5"/>
-    <col min="7" max="7" width="3.7265625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="3.54296875" customWidth="1"/>
-    <col min="15" max="15" width="4.7265625" customWidth="1"/>
-    <col min="19" max="19" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="6" width="8.77734375" style="5"/>
+    <col min="7" max="7" width="3.77734375" style="5" customWidth="1"/>
+    <col min="11" max="11" width="3.5546875" customWidth="1"/>
+    <col min="15" max="15" width="4.77734375" customWidth="1"/>
+    <col min="19" max="19" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="4.08984375" customWidth="1"/>
-    <col min="23" max="23" width="6.81640625" customWidth="1"/>
-    <col min="24" max="24" width="7.36328125" customWidth="1"/>
-    <col min="25" max="25" width="6.6328125" customWidth="1"/>
-    <col min="26" max="26" width="11.1796875" customWidth="1"/>
-    <col min="31" max="31" width="4.08984375" customWidth="1"/>
-    <col min="33" max="33" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.109375" customWidth="1"/>
+    <col min="23" max="23" width="6.77734375" customWidth="1"/>
+    <col min="24" max="24" width="7.33203125" customWidth="1"/>
+    <col min="25" max="25" width="6.6640625" customWidth="1"/>
+    <col min="26" max="26" width="11.21875" customWidth="1"/>
+    <col min="31" max="31" width="4.109375" customWidth="1"/>
+    <col min="33" max="33" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
       <c r="K1" s="35"/>
-      <c r="L1" s="43" t="s">
+      <c r="L1" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="P1" s="43" t="s">
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="P1" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="Q1" s="43"/>
-      <c r="R1" s="43"/>
-      <c r="S1" s="43"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="W1" s="43" t="s">
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="W1" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="X1" s="43"/>
-      <c r="Y1" s="43"/>
-      <c r="Z1" s="43"/>
-      <c r="AA1" s="43"/>
-      <c r="AB1" s="43"/>
-      <c r="AC1" s="43"/>
-      <c r="AD1" s="43"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
+      <c r="AA1" s="44"/>
+      <c r="AB1" s="44"/>
+      <c r="AC1" s="44"/>
+      <c r="AD1" s="44"/>
       <c r="AE1" s="2"/>
       <c r="AF1" s="35">
         <v>345</v>
@@ -5727,7 +5796,7 @@
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="4" t="s">
@@ -6651,417 +6720,417 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{882535D5-A2FC-450C-9372-2FDC3B63387E}">
   <dimension ref="A1:A81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="44"/>
+    <col min="1" max="16384" width="8.77734375" style="43"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="43" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="43" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="43" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="43" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="43" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="43" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="43" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="44" t="s">
+      <c r="A8" s="43" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="44" t="s">
+      <c r="A9" s="43" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="43" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="43" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="43" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="43" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="43" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="43" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="43" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="43" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="43" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="43" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="43" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="43" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="44" t="s">
+      <c r="A22" s="43" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="43" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="44" t="s">
+      <c r="A24" s="43" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="44" t="s">
+      <c r="A25" s="43" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="44" t="s">
+      <c r="A26" s="43" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="44" t="s">
+      <c r="A27" s="43" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="44" t="s">
+      <c r="A28" s="43" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="43" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="44" t="s">
+      <c r="A30" s="43" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="44" t="s">
+      <c r="A31" s="43" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="44" t="s">
+      <c r="A32" s="43" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="44" t="s">
+      <c r="A33" s="43" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="44" t="s">
+      <c r="A34" s="43" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="44" t="s">
+      <c r="A35" s="43" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="44" t="s">
+      <c r="A36" s="43" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" s="44" t="s">
+      <c r="A37" s="43" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="44" t="s">
+      <c r="A38" s="43" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="44" t="s">
+      <c r="A39" s="43" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="44" t="s">
+      <c r="A40" s="43" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="44" t="s">
+      <c r="A41" s="43" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="44" t="s">
+      <c r="A42" s="43" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="44" t="s">
+      <c r="A43" s="43" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="44" t="s">
+      <c r="A44" s="43" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="44" t="s">
+      <c r="A45" s="43" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="44" t="s">
+      <c r="A46" s="43" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="44" t="s">
+      <c r="A47" s="43" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="44" t="s">
+      <c r="A48" s="43" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="44" t="s">
+      <c r="A49" s="43" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="44" t="s">
+      <c r="A50" s="43" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="44" t="s">
+      <c r="A51" s="43" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="44" t="s">
+      <c r="A52" s="43" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="44" t="s">
+      <c r="A53" s="43" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="44" t="s">
+      <c r="A54" s="43" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="44" t="s">
+      <c r="A55" s="43" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="44" t="s">
+      <c r="A56" s="43" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="44" t="s">
+      <c r="A57" s="43" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="44" t="s">
+      <c r="A58" s="43" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="44" t="s">
+      <c r="A59" s="43" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="44" t="s">
+      <c r="A60" s="43" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="44" t="s">
+      <c r="A61" s="43" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="44" t="s">
+      <c r="A62" s="43" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="44" t="s">
+      <c r="A63" s="43" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="44" t="s">
+      <c r="A64" s="43" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" s="44" t="s">
+      <c r="A65" s="43" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="44" t="s">
+      <c r="A66" s="43" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" s="44" t="s">
+      <c r="A67" s="43" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="44" t="s">
+      <c r="A68" s="43" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="44" t="s">
+      <c r="A69" s="43" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="44" t="s">
+      <c r="A70" s="43" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="44" t="s">
+      <c r="A71" s="43" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="44" t="s">
+      <c r="A72" s="43" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="44" t="s">
+      <c r="A73" s="43" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="44" t="s">
+      <c r="A74" s="43" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="44" t="s">
+      <c r="A75" s="43" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="76" spans="1:1">
-      <c r="A76" s="44" t="s">
+      <c r="A76" s="43" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="77" spans="1:1">
-      <c r="A77" s="44" t="s">
+      <c r="A77" s="43" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="78" spans="1:1">
-      <c r="A78" s="44" t="s">
+      <c r="A78" s="43" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="79" spans="1:1">
-      <c r="A79" s="44" t="s">
+      <c r="A79" s="43" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="80" spans="1:1">
-      <c r="A80" s="44" t="s">
+      <c r="A80" s="43" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="81" spans="1:1">
-      <c r="A81" s="44" t="s">
+      <c r="A81" s="43" t="s">
         <v>169</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added COMTRADE recorder and StudyScript.dwj for WindSystem
</commit_message>
<xml_diff>
--- a/emt-bootcamp/Support/EMTBootCamp.xlsx
+++ b/emt-bootcamp/Support/EMTBootCamp.xlsx
@@ -8,42 +8,53 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\i2x\emt-bootcamp\Support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780D16BA-B075-4B4B-8308-0579915B75EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65304C97-45EE-4FB8-B75A-66019EC87A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="11232" activeTab="3" xr2:uid="{A8C2E3F1-142E-440E-A762-DE7B4CF8E5D3}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9024" activeTab="1" xr2:uid="{A8C2E3F1-142E-440E-A762-DE7B4CF8E5D3}"/>
   </bookViews>
   <sheets>
     <sheet name="COMTRADE" sheetId="1" r:id="rId1"/>
-    <sheet name="Source" sheetId="2" r:id="rId2"/>
-    <sheet name="Weak" sheetId="3" r:id="rId3"/>
-    <sheet name="StepSCR" sheetId="4" r:id="rId4"/>
-    <sheet name="IEEE39m" sheetId="5" r:id="rId5"/>
-    <sheet name="HCA" sheetId="6" r:id="rId6"/>
-    <sheet name="HCA_Upgrades" sheetId="7" r:id="rId7"/>
+    <sheet name="COMTRADE_39" sheetId="8" r:id="rId2"/>
+    <sheet name="Source" sheetId="2" r:id="rId3"/>
+    <sheet name="Weak" sheetId="3" r:id="rId4"/>
+    <sheet name="StepSCR" sheetId="4" r:id="rId5"/>
+    <sheet name="IEEE39m" sheetId="5" r:id="rId6"/>
+    <sheet name="HCA" sheetId="6" r:id="rId7"/>
+    <sheet name="HCA_Upgrades" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
+    <definedName name="Dmax" localSheetId="1">COMTRADE_39!$N$2</definedName>
     <definedName name="Dmax">COMTRADE!$N$2</definedName>
+    <definedName name="Dmin" localSheetId="1">COMTRADE_39!$N$1</definedName>
     <definedName name="Dmin">COMTRADE!$N$1</definedName>
+    <definedName name="Ibase" localSheetId="1">COMTRADE_39!$N$5</definedName>
     <definedName name="Ibase">COMTRADE!$N$5</definedName>
+    <definedName name="IpuMax" localSheetId="1">COMTRADE_39!$N$10</definedName>
     <definedName name="IpuMax">COMTRADE!$N$10</definedName>
+    <definedName name="Iscale" localSheetId="1">COMTRADE_39!$N$7</definedName>
     <definedName name="Iscale">COMTRADE!$N$7</definedName>
     <definedName name="kvb">IEEE39m!$AF$1</definedName>
     <definedName name="mips">IEEE39m!$AJ$1</definedName>
     <definedName name="sb">IEEE39m!$AG$1</definedName>
+    <definedName name="Splant" localSheetId="1">COMTRADE_39!$N$3</definedName>
     <definedName name="Splant">COMTRADE!$N$3</definedName>
+    <definedName name="SpuMax" localSheetId="1">COMTRADE_39!$N$11</definedName>
     <definedName name="SpuMax">COMTRADE!$N$11</definedName>
+    <definedName name="Sscale" localSheetId="1">COMTRADE_39!$N$8</definedName>
     <definedName name="Sscale">COMTRADE!$N$8</definedName>
+    <definedName name="Vpoc" localSheetId="1">COMTRADE_39!$N$4</definedName>
     <definedName name="Vpoc">COMTRADE!$N$4</definedName>
+    <definedName name="VpuMax" localSheetId="1">COMTRADE_39!$N$9</definedName>
     <definedName name="VpuMax">COMTRADE!$N$9</definedName>
+    <definedName name="Vscale" localSheetId="1">COMTRADE_39!$N$6</definedName>
     <definedName name="Vscale">COMTRADE!$N$6</definedName>
     <definedName name="wb">IEEE39m!$AH$1</definedName>
-    <definedName name="XS" localSheetId="3">StepSCR!$K$6</definedName>
-    <definedName name="XS" localSheetId="2">Weak!$F$5</definedName>
+    <definedName name="XS" localSheetId="4">StepSCR!$K$6</definedName>
+    <definedName name="XS" localSheetId="3">Weak!$F$5</definedName>
     <definedName name="XS">Source!$F$5</definedName>
     <definedName name="zb">IEEE39m!$AI$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -64,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="180">
   <si>
     <t>Name</t>
   </si>
@@ -806,7 +817,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -913,6 +924,9 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1233,7 +1247,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1744,6 +1758,334 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34CE9B6F-BF56-4B7C-AE26-6892E945C0B3}">
+  <dimension ref="A1:N11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="4" max="4" width="8.77734375" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" customWidth="1"/>
+    <col min="12" max="12" width="5.77734375" customWidth="1"/>
+    <col min="13" max="13" width="9.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="28.8">
+      <c r="A1" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="9">
+        <v>-32767</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="12"/>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="9">
+        <v>32767</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="12"/>
+      <c r="M3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="10">
+        <v>300000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="12"/>
+      <c r="M4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="10">
+        <v>345000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="12"/>
+      <c r="M5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5">
+        <f>Splant/SQRT(3)/Vpoc</f>
+        <v>502.04371233880505</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="12"/>
+      <c r="M6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="12"/>
+      <c r="M7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="16">
+        <v>0</v>
+      </c>
+      <c r="G8" s="17">
+        <f>Vpoc*Vscale*VpuMax/SQRT(3)</f>
+        <v>398371.68574084179</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" ref="H2:H11" si="0">(G8-F8)/(Dmax-Dmin)</f>
+        <v>6.0788550331254276</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" ref="I2:I11" si="1">G8-H8*Dmax</f>
+        <v>199185.84287042089</v>
+      </c>
+      <c r="J8" s="12">
+        <v>1000</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="M8" t="s">
+        <v>31</v>
+      </c>
+      <c r="N8" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="3">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="19">
+        <f>-G9</f>
+        <v>-900000000</v>
+      </c>
+      <c r="G9" s="18">
+        <f>Splant*Sscale*SpuMax</f>
+        <v>900000000</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" si="0"/>
+        <v>27466.658528397475</v>
+      </c>
+      <c r="I9" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="12">
+        <v>1000000</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="M9" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="3">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="19">
+        <f>-G10</f>
+        <v>-900000000</v>
+      </c>
+      <c r="G10" s="19">
+        <f>G$9</f>
+        <v>900000000</v>
+      </c>
+      <c r="H10" s="5">
+        <f t="shared" si="0"/>
+        <v>27466.658528397475</v>
+      </c>
+      <c r="I10" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="12">
+        <v>1000000</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="M10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N10" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="12"/>
+      <c r="M11" t="s">
+        <v>34</v>
+      </c>
+      <c r="N11" s="9">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7143908-12DE-459A-B5BB-96ECEF0A7C1B}">
   <dimension ref="A1:F9"/>
   <sheetViews>
@@ -1893,7 +2235,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE8CDAB3-5235-4A87-8D47-F5FCC0EB49C6}">
   <dimension ref="A1:F9"/>
   <sheetViews>
@@ -2043,11 +2385,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70A51ED4-A577-4B06-8042-A04C86E2D43B}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -2060,14 +2402,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44" t="s">
+      <c r="E1" s="45"/>
+      <c r="F1" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="44"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="4" t="s">
@@ -2443,7 +2785,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F98AF1C0-18B6-49C9-8A8E-53F5401F1E81}">
   <dimension ref="A1:AJ48"/>
   <sheetViews>
@@ -2470,44 +2812,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="44" t="s">
+      <c r="H1" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
       <c r="K1" s="35"/>
-      <c r="L1" s="44" t="s">
+      <c r="L1" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="P1" s="44" t="s">
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="P1" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="W1" s="44" t="s">
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="W1" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
-      <c r="AA1" s="44"/>
-      <c r="AB1" s="44"/>
-      <c r="AC1" s="44"/>
-      <c r="AD1" s="44"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="45"/>
+      <c r="AA1" s="45"/>
+      <c r="AB1" s="45"/>
+      <c r="AC1" s="45"/>
+      <c r="AD1" s="45"/>
       <c r="AE1" s="2"/>
       <c r="AF1" s="35">
         <v>345</v>
@@ -5788,7 +6130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6054D9DB-8259-4710-A733-63A2E8D1DD9B}">
   <dimension ref="A1:I32"/>
   <sheetViews>
@@ -6716,7 +7058,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{882535D5-A2FC-450C-9372-2FDC3B63387E}">
   <dimension ref="A1:A81"/>
   <sheetViews>

</xml_diff>